<commit_message>
unidades de almacenamiento y configuracion lan
</commit_message>
<xml_diff>
--- a/docs/protocols_suite.xlsx
+++ b/docs/protocols_suite.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\networks\CISCO\saves\ccna-s10\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFCB8F1F-AACF-4137-B893-3FD4825218A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B44CCA8-C5F6-4AAE-9DB7-EA54421CB024}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{F2A32163-0D52-4F0A-8C5D-6317EB95D18F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{F2A32163-0D52-4F0A-8C5D-6317EB95D18F}"/>
   </bookViews>
   <sheets>
     <sheet name="modelos" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="75">
   <si>
     <t>OSI de ISO</t>
   </si>
@@ -119,6 +119,150 @@
   </si>
   <si>
     <t>100BaseT, 100BaseTx, 100BaseFx, 100BaseCx</t>
+  </si>
+  <si>
+    <t>bit</t>
+  </si>
+  <si>
+    <t>Binary Digit</t>
+  </si>
+  <si>
+    <t>U. Minima</t>
+  </si>
+  <si>
+    <t>ALMACENAMIENTO</t>
+  </si>
+  <si>
+    <t>ANCHO DE BANDA</t>
+  </si>
+  <si>
+    <t>Unidad</t>
+  </si>
+  <si>
+    <t>Equivalencia</t>
+  </si>
+  <si>
+    <t>Exponente</t>
+  </si>
+  <si>
+    <t>Byte</t>
+  </si>
+  <si>
+    <t>8 bits</t>
+  </si>
+  <si>
+    <t>10^0</t>
+  </si>
+  <si>
+    <t>KiloByte</t>
+  </si>
+  <si>
+    <t>10^3</t>
+  </si>
+  <si>
+    <t>10^6</t>
+  </si>
+  <si>
+    <t>10^9</t>
+  </si>
+  <si>
+    <t>10^12</t>
+  </si>
+  <si>
+    <t>10^15</t>
+  </si>
+  <si>
+    <t>10^18</t>
+  </si>
+  <si>
+    <t>10^21</t>
+  </si>
+  <si>
+    <t>10^24</t>
+  </si>
+  <si>
+    <t>10^27</t>
+  </si>
+  <si>
+    <t>10^30</t>
+  </si>
+  <si>
+    <t>10^33</t>
+  </si>
+  <si>
+    <t>MegaByte</t>
+  </si>
+  <si>
+    <t>1000B</t>
+  </si>
+  <si>
+    <t>1000KB</t>
+  </si>
+  <si>
+    <t>GigaByte</t>
+  </si>
+  <si>
+    <t>1000MB</t>
+  </si>
+  <si>
+    <t>TeraByte</t>
+  </si>
+  <si>
+    <t>1000GB</t>
+  </si>
+  <si>
+    <t>PetaByte</t>
+  </si>
+  <si>
+    <t>ExaByte</t>
+  </si>
+  <si>
+    <t>ZettaByte</t>
+  </si>
+  <si>
+    <t>YottaByte</t>
+  </si>
+  <si>
+    <t>BrontoByte</t>
+  </si>
+  <si>
+    <t>GeopByte</t>
+  </si>
+  <si>
+    <t>SaganByte</t>
+  </si>
+  <si>
+    <t>1000TB</t>
+  </si>
+  <si>
+    <t>1000PB</t>
+  </si>
+  <si>
+    <t>1000XB</t>
+  </si>
+  <si>
+    <t>1000ZB</t>
+  </si>
+  <si>
+    <t>1000YB</t>
+  </si>
+  <si>
+    <t>1000BB</t>
+  </si>
+  <si>
+    <t>1000GeB</t>
+  </si>
+  <si>
+    <t>KiB</t>
+  </si>
+  <si>
+    <t>GiB</t>
+  </si>
+  <si>
+    <t>MiB</t>
+  </si>
+  <si>
+    <t>TiB</t>
   </si>
 </sst>
 </file>
@@ -234,8 +378,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -292,6 +442,9 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
@@ -616,8 +769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26B8B09C-E1B7-4EAF-8A56-2848F2F39911}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,113 +779,114 @@
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="41.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="14" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="17" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="17"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="19"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="17"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="19"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="8" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="6"/>
+      <c r="D8" s="8"/>
     </row>
     <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="20" t="s">
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="22" t="s">
         <v>6</v>
       </c>
     </row>
@@ -750,12 +904,211 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67F5B955-0179-44D1-8995-F7853F4C3651}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6:D9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="E3:G3"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
tipos de comunicacion y normas tia568a y 568b
</commit_message>
<xml_diff>
--- a/docs/protocols_suite.xlsx
+++ b/docs/protocols_suite.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\networks\CISCO\saves\ccna-s10\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B44CCA8-C5F6-4AAE-9DB7-EA54421CB024}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FBCE632-69B4-4497-8B49-EB77B1811309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{F2A32163-0D52-4F0A-8C5D-6317EB95D18F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{F2A32163-0D52-4F0A-8C5D-6317EB95D18F}"/>
   </bookViews>
   <sheets>
     <sheet name="modelos" sheetId="1" r:id="rId1"/>
     <sheet name="unidades" sheetId="2" r:id="rId2"/>
+    <sheet name="fisica" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">modelos!$C$1:$C$14</definedName>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="144">
   <si>
     <t>OSI de ISO</t>
   </si>
@@ -142,9 +143,6 @@
     <t>Equivalencia</t>
   </si>
   <si>
-    <t>Exponente</t>
-  </si>
-  <si>
     <t>Byte</t>
   </si>
   <si>
@@ -263,13 +261,227 @@
   </si>
   <si>
     <t>TiB</t>
+  </si>
+  <si>
+    <t>Real</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>PiB</t>
+  </si>
+  <si>
+    <t>ZiB</t>
+  </si>
+  <si>
+    <t>YiB</t>
+  </si>
+  <si>
+    <t>BiB</t>
+  </si>
+  <si>
+    <t>XiB</t>
+  </si>
+  <si>
+    <t>GeiB</t>
+  </si>
+  <si>
+    <t>SiB</t>
+  </si>
+  <si>
+    <t>Kilobits/second</t>
+  </si>
+  <si>
+    <t>bits/second</t>
+  </si>
+  <si>
+    <t>Megabits/second</t>
+  </si>
+  <si>
+    <t>Gigabits/second</t>
+  </si>
+  <si>
+    <t>Terabit/second</t>
+  </si>
+  <si>
+    <t>1000bps</t>
+  </si>
+  <si>
+    <t>1000Gbps</t>
+  </si>
+  <si>
+    <t>1000Mbps</t>
+  </si>
+  <si>
+    <t>1000Kbps</t>
+  </si>
+  <si>
+    <t>Exp.</t>
+  </si>
+  <si>
+    <t>Exp</t>
+  </si>
+  <si>
+    <t>Equiv</t>
+  </si>
+  <si>
+    <t>FRECUENCIA</t>
+  </si>
+  <si>
+    <t>Hertz</t>
+  </si>
+  <si>
+    <t>KiloHertz</t>
+  </si>
+  <si>
+    <t>MegaHertz</t>
+  </si>
+  <si>
+    <t>GigaHertz</t>
+  </si>
+  <si>
+    <t>TeraHertz</t>
+  </si>
+  <si>
+    <t>1 ciclo por seg</t>
+  </si>
+  <si>
+    <t>1 bit por seg</t>
+  </si>
+  <si>
+    <t>1000Hz</t>
+  </si>
+  <si>
+    <t>1000KHz</t>
+  </si>
+  <si>
+    <t>1000MHz</t>
+  </si>
+  <si>
+    <t>1000GHz</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>AM</t>
+  </si>
+  <si>
+    <t>FM</t>
+  </si>
+  <si>
+    <t>PM</t>
+  </si>
+  <si>
+    <t>Señal</t>
+  </si>
+  <si>
+    <t>Carrier</t>
+  </si>
+  <si>
+    <t>Definicion</t>
+  </si>
+  <si>
+    <t>Amplitud Modulada</t>
+  </si>
+  <si>
+    <t>Frecuencia Modulada</t>
+  </si>
+  <si>
+    <t>Modulacion de Fase</t>
+  </si>
+  <si>
+    <t>Señal Portadora</t>
+  </si>
+  <si>
+    <t>TIA 568A</t>
+  </si>
+  <si>
+    <t>TIA568B</t>
+  </si>
+  <si>
+    <t>B.Verde</t>
+  </si>
+  <si>
+    <t>Verde</t>
+  </si>
+  <si>
+    <t>B.Naranja</t>
+  </si>
+  <si>
+    <t>Azul</t>
+  </si>
+  <si>
+    <t>B.Azul</t>
+  </si>
+  <si>
+    <t>Naranja</t>
+  </si>
+  <si>
+    <t>B.Marron</t>
+  </si>
+  <si>
+    <t>Marron</t>
+  </si>
+  <si>
+    <t>Rx</t>
+  </si>
+  <si>
+    <t>Tx</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>Simplex</t>
+  </si>
+  <si>
+    <t>Uno Envia o Recibe</t>
+  </si>
+  <si>
+    <t>Uno Envia, no Recibe</t>
+  </si>
+  <si>
+    <t>Uno Envia y Recibe</t>
+  </si>
+  <si>
+    <t>Muchos a Muchos</t>
+  </si>
+  <si>
+    <t>Comunicación</t>
+  </si>
+  <si>
+    <t>Half Duplex</t>
+  </si>
+  <si>
+    <t>Full Duplex</t>
+  </si>
+  <si>
+    <t>Full Full Duplex</t>
+  </si>
+  <si>
+    <t>Pin</t>
+  </si>
+  <si>
+    <t>Fibra</t>
+  </si>
+  <si>
+    <t>MMF</t>
+  </si>
+  <si>
+    <t>SMF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -298,8 +510,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -347,8 +566,62 @@
         <bgColor theme="4"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD2906C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -374,18 +647,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -396,9 +687,6 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -426,35 +714,121 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Millares" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFD2906C"/>
       <color rgb="FFCC3300"/>
       <color rgb="FFA50021"/>
     </mruColors>
@@ -468,6 +842,245 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>877303</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>80213</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>45119</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>125329</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Conector recto 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF5C6DE5-FA91-42B0-8CBD-2B847EBBF78B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="877303" y="270713"/>
+          <a:ext cx="581527" cy="426116"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:schemeClr val="accent2">
+              <a:lumMod val="60000"/>
+              <a:lumOff val="40000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>907382</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>80213</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>25066</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>155408</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Conector recto 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB5CF41A-E893-4BC5-9178-23D49FBE38EB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="907382" y="461213"/>
+          <a:ext cx="531395" cy="837195"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:schemeClr val="accent2">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>817145</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>40105</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>72189</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>107282</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Conector recto 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47BDE5BB-F2F6-430D-9AC6-1CBA62A21E77}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="817145" y="230605"/>
+          <a:ext cx="668755" cy="448177"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="60000"/>
+              <a:lumOff val="40000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>100263</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>55144</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>130342</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Conector recto 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F281630-8200-43F2-8EED-0F49CDDE1B4C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="952500" y="481263"/>
+          <a:ext cx="516355" cy="792079"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -769,7 +1382,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26B8B09C-E1B7-4EAF-8A56-2848F2F39911}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C4"/>
     </sheetView>
   </sheetViews>
@@ -783,110 +1396,110 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="12" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="18" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="19"/>
-      <c r="C3" s="20"/>
+      <c r="C3" s="22"/>
       <c r="D3" s="19"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="19"/>
-      <c r="C4" s="20"/>
+      <c r="C4" s="22"/>
       <c r="D4" s="19"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="20" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="8"/>
+      <c r="D8" s="20"/>
     </row>
     <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="22" t="s">
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="16" t="s">
         <v>6</v>
       </c>
     </row>
@@ -904,211 +1517,661 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67F5B955-0179-44D1-8995-F7853F4C3651}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:D9"/>
+    <sheetView topLeftCell="G4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4" customWidth="1"/>
+    <col min="10" max="17" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="D1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1" s="28"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="27"/>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="E3" s="2" t="s">
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="F3" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="H4" s="38" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1" t="s">
+      <c r="B5" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="E5" s="17"/>
+      <c r="F5" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="G5" s="39" t="s">
+        <v>102</v>
+      </c>
+      <c r="H5" s="39" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" s="17"/>
+      <c r="F6" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="G6" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="H6" s="31" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" s="17"/>
+      <c r="F7" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="G7" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="H7" s="30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" s="17"/>
+      <c r="F8" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="G8" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="H8" s="31" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="E9" s="17"/>
+      <c r="F9" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="G9" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="H9" s="32" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="E10" s="17"/>
+      <c r="F10" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" s="17"/>
+      <c r="F11" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G11" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="23" t="s">
+      <c r="H11" s="29" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="E12" s="17"/>
+      <c r="F12" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="G12" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="H12" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="23" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="E13" s="17"/>
+      <c r="F13" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="G13" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="H13" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" s="23" t="s">
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="E14" s="17"/>
+      <c r="F14" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="G14" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="H14" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="23" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" s="23" t="s">
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="37" t="s">
+        <v>81</v>
+      </c>
+      <c r="E15" s="17"/>
+      <c r="F15" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="G15" s="31" t="s">
+        <v>105</v>
+      </c>
+      <c r="H15" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="23" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="C8" s="23" t="s">
+    </row>
+    <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="E16" s="17"/>
+      <c r="F16" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="G16" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="H16" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="23" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="B9" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="23" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="B10" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="B11" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="C11" s="23" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="B12" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="B13" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="C13" s="23" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="B14" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="C14" s="23" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="B15" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="C15" s="23" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="B16" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="C16" s="23" t="s">
-        <v>49</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A3:C3"/>
-    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="F10:H10"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB50611C-C95E-47CD-8ED7-7DBE740143C6}">
+  <dimension ref="A1:M25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" style="17" customWidth="1"/>
+    <col min="4" max="4" width="3.28515625" style="40" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="40" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" style="40" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" style="40" customWidth="1"/>
+    <col min="8" max="8" width="3" style="40" customWidth="1"/>
+    <col min="9" max="10" width="9.42578125" style="40" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" style="41" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E1" s="42" t="s">
+        <v>141</v>
+      </c>
+      <c r="F1" s="42" t="s">
+        <v>143</v>
+      </c>
+      <c r="G1" s="53" t="s">
+        <v>142</v>
+      </c>
+      <c r="K1" s="40"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="44" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" s="46" t="s">
+        <v>122</v>
+      </c>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="45" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C3" s="49" t="s">
+        <v>125</v>
+      </c>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="40"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="46" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C4" s="44" t="s">
+        <v>120</v>
+      </c>
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
+      <c r="M4" s="40"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="47" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="47" t="s">
+        <v>123</v>
+      </c>
+      <c r="K5" s="40"/>
+      <c r="L5" s="40"/>
+      <c r="M5" s="40"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="48" t="s">
+        <v>124</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="48" t="s">
+        <v>124</v>
+      </c>
+      <c r="K6" s="40"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="40"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="49" t="s">
+        <v>125</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C7" s="45" t="s">
+        <v>121</v>
+      </c>
+      <c r="K7" s="40"/>
+      <c r="L7" s="40"/>
+      <c r="M7" s="40"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="50" t="s">
+        <v>126</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="50" t="s">
+        <v>126</v>
+      </c>
+      <c r="K8" s="40"/>
+      <c r="L8" s="40"/>
+      <c r="M8" s="40"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="51" t="s">
+        <v>127</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="51" t="s">
+        <v>127</v>
+      </c>
+      <c r="K9" s="40"/>
+      <c r="L9" s="40"/>
+      <c r="M9" s="40"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K10" s="40"/>
+      <c r="L10" s="40"/>
+      <c r="M10" s="40"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="B11" s="43" t="s">
+        <v>136</v>
+      </c>
+      <c r="C11" s="43"/>
+      <c r="E11" t="s">
+        <v>111</v>
+      </c>
+      <c r="F11" t="s">
+        <v>113</v>
+      </c>
+      <c r="K11" s="40"/>
+      <c r="L11" s="40"/>
+      <c r="M11" s="40"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="B12" s="43" t="s">
+        <v>133</v>
+      </c>
+      <c r="C12" s="43"/>
+      <c r="E12" t="s">
+        <v>112</v>
+      </c>
+      <c r="F12" t="s">
+        <v>117</v>
+      </c>
+      <c r="K12" s="40"/>
+      <c r="L12" s="40"/>
+      <c r="M12" s="40"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="B13" s="43" t="s">
+        <v>132</v>
+      </c>
+      <c r="C13" s="43"/>
+      <c r="E13" t="s">
+        <v>108</v>
+      </c>
+      <c r="F13" t="s">
+        <v>114</v>
+      </c>
+      <c r="K13" s="40"/>
+      <c r="L13" s="40"/>
+      <c r="M13" s="40"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="B14" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="C14" s="43"/>
+      <c r="E14" t="s">
+        <v>109</v>
+      </c>
+      <c r="F14" t="s">
+        <v>115</v>
+      </c>
+      <c r="K14" s="40"/>
+      <c r="L14" s="40"/>
+      <c r="M14" s="40"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="24" t="s">
+        <v>139</v>
+      </c>
+      <c r="B15" s="43" t="s">
+        <v>135</v>
+      </c>
+      <c r="C15" s="43"/>
+      <c r="E15" t="s">
+        <v>110</v>
+      </c>
+      <c r="F15" t="s">
+        <v>116</v>
+      </c>
+      <c r="K15" s="40"/>
+      <c r="L15" s="40"/>
+      <c r="M15" s="40"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C16" s="52"/>
+      <c r="K16" s="40"/>
+      <c r="L16" s="40"/>
+      <c r="M16" s="40"/>
+    </row>
+    <row r="17" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C17" s="52"/>
+      <c r="K17" s="40"/>
+    </row>
+    <row r="18" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C18" s="52"/>
+      <c r="K18" s="40"/>
+    </row>
+    <row r="19" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C19" s="52"/>
+    </row>
+    <row r="20" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C20" s="52"/>
+    </row>
+    <row r="21" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C21" s="52"/>
+    </row>
+    <row r="22" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C22" s="52"/>
+    </row>
+    <row r="23" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C23" s="52"/>
+    </row>
+    <row r="24" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C24" s="52"/>
+    </row>
+    <row r="25" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C25" s="52"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
tipos de conectores y caracterificas smf mmf
</commit_message>
<xml_diff>
--- a/docs/protocols_suite.xlsx
+++ b/docs/protocols_suite.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\networks\CISCO\saves\ccna-s10\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FBCE632-69B4-4497-8B49-EB77B1811309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73144611-A555-4C54-BF09-6F8B1CB93B49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{F2A32163-0D52-4F0A-8C5D-6317EB95D18F}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="modelos" sheetId="1" r:id="rId1"/>
     <sheet name="unidades" sheetId="2" r:id="rId2"/>
     <sheet name="fisica" sheetId="3" r:id="rId3"/>
+    <sheet name="enlace" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">modelos!$C$1:$C$14</definedName>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="191">
   <si>
     <t>OSI de ISO</t>
   </si>
@@ -471,6 +472,147 @@
   </si>
   <si>
     <t>SMF</t>
+  </si>
+  <si>
+    <t>tipo</t>
+  </si>
+  <si>
+    <t>Monomodo</t>
+  </si>
+  <si>
+    <t>Multimodo</t>
+  </si>
+  <si>
+    <t>luz</t>
+  </si>
+  <si>
+    <t>laser</t>
+  </si>
+  <si>
+    <t>led</t>
+  </si>
+  <si>
+    <t>rango</t>
+  </si>
+  <si>
+    <t>200km</t>
+  </si>
+  <si>
+    <t>2km</t>
+  </si>
+  <si>
+    <t>nucleo</t>
+  </si>
+  <si>
+    <t>9 micrones</t>
+  </si>
+  <si>
+    <t>60 micrones</t>
+  </si>
+  <si>
+    <t>capac</t>
+  </si>
+  <si>
+    <t>10Gbps</t>
+  </si>
+  <si>
+    <t>100Gbps</t>
+  </si>
+  <si>
+    <t>ventaja</t>
+  </si>
+  <si>
+    <t>contra</t>
+  </si>
+  <si>
+    <t>uso</t>
+  </si>
+  <si>
+    <t>Electronica</t>
+  </si>
+  <si>
+    <t>Economica</t>
+  </si>
+  <si>
+    <t>Hogares</t>
+  </si>
+  <si>
+    <t>Empresas</t>
+  </si>
+  <si>
+    <t>Conector</t>
+  </si>
+  <si>
+    <t>Terminacion</t>
+  </si>
+  <si>
+    <t>FC</t>
+  </si>
+  <si>
+    <t>ST</t>
+  </si>
+  <si>
+    <t>SC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>Ferrule Connector</t>
+  </si>
+  <si>
+    <t>Straigth Tip</t>
+  </si>
+  <si>
+    <t>Suscriber Connector</t>
+  </si>
+  <si>
+    <t>Lucent Connector</t>
+  </si>
+  <si>
+    <t>PC</t>
+  </si>
+  <si>
+    <t>UPC</t>
+  </si>
+  <si>
+    <t>APC</t>
+  </si>
+  <si>
+    <t>Physical Connector</t>
+  </si>
+  <si>
+    <t>Ultra Physical Connector</t>
+  </si>
+  <si>
+    <t>Angled Physical Connector</t>
+  </si>
+  <si>
+    <t>Problemas</t>
+  </si>
+  <si>
+    <t>EMI</t>
+  </si>
+  <si>
+    <t>RFI</t>
+  </si>
+  <si>
+    <t>CrossTalk</t>
+  </si>
+  <si>
+    <t>Colision</t>
+  </si>
+  <si>
+    <t>Interf. Electromagnetica</t>
+  </si>
+  <si>
+    <t>Interf. Por Radiofrecuencia</t>
+  </si>
+  <si>
+    <t>Diafonia</t>
+  </si>
+  <si>
+    <t>Choque datos / Señales</t>
   </si>
 </sst>
 </file>
@@ -672,7 +814,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -740,9 +882,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -783,12 +922,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -816,15 +949,65 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -849,7 +1032,7 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>877303</xdr:colOff>
+      <xdr:colOff>917408</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>80213</xdr:rowOff>
     </xdr:from>
@@ -857,7 +1040,7 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>45119</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>125329</xdr:rowOff>
+      <xdr:rowOff>50132</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -872,8 +1055,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="877303" y="270713"/>
-          <a:ext cx="581527" cy="426116"/>
+          <a:off x="917408" y="270713"/>
+          <a:ext cx="1112922" cy="350919"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1025,9 +1208,9 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>952500</xdr:colOff>
+      <xdr:colOff>972553</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>100263</xdr:rowOff>
+      <xdr:rowOff>55145</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
@@ -1048,8 +1231,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="952500" y="481263"/>
-          <a:ext cx="516355" cy="792079"/>
+          <a:off x="972553" y="436145"/>
+          <a:ext cx="1067802" cy="837197"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1081,6 +1264,40 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C2C01944-185D-43BF-8A62-D61C3ABD55B5}" name="Tabla3" displayName="Tabla3" ref="E1:G9" totalsRowShown="0" dataDxfId="0">
+  <autoFilter ref="E1:G9" xr:uid="{C2C01944-185D-43BF-8A62-D61C3ABD55B5}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{8079FA69-59E6-4C3F-8414-22F5F08661F0}" name="Fibra" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{51C999F5-4709-4731-A8C0-5DF1FB13B02F}" name="SMF" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{D64CF8DA-A5E3-4CD8-B0D7-1B8FF7A3D8F6}" name="MMF" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{C78321D3-CCFD-43D7-8B50-0C45EEA5B1E7}" name="Tabla6" displayName="Tabla6" ref="I1:J5" totalsRowShown="0">
+  <autoFilter ref="I1:J5" xr:uid="{C78321D3-CCFD-43D7-8B50-0C45EEA5B1E7}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{08E9B9E5-F910-401F-93ED-C04AD37535EF}" name="Conector"/>
+    <tableColumn id="2" xr3:uid="{D5269F62-4479-4F3D-A5D4-C1ED26AF7B5B}" name="Definicion"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{52135C1B-9F95-4015-B02C-B87CD34D509E}" name="Tabla8" displayName="Tabla8" ref="I6:J9" totalsRowShown="0">
+  <autoFilter ref="I6:J9" xr:uid="{52135C1B-9F95-4015-B02C-B87CD34D509E}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{543EB15E-529C-425D-915D-1E4596E25696}" name="Terminacion"/>
+    <tableColumn id="2" xr3:uid="{BC2527C8-7181-4C90-8F5A-90CCE514EF2C}" name="Definicion"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1519,7 +1736,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67F5B955-0179-44D1-8995-F7853F4C3651}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView topLeftCell="G4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
@@ -1550,10 +1767,10 @@
       <c r="D1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="F1" s="28"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="26"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="23" t="s">
@@ -1568,160 +1785,160 @@
       <c r="H3" s="23"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="33" t="s">
         <v>74</v>
       </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="38" t="s">
+      <c r="F4" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="38" t="s">
+      <c r="G4" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="38" t="s">
+      <c r="H4" s="37" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="D5" s="34" t="s">
         <v>75</v>
       </c>
       <c r="E5" s="17"/>
-      <c r="F5" s="39" t="s">
+      <c r="F5" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="G5" s="39" t="s">
+      <c r="G5" s="38" t="s">
         <v>102</v>
       </c>
-      <c r="H5" s="39" t="s">
+      <c r="H5" s="38" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="36" t="s">
+      <c r="D6" s="35" t="s">
         <v>70</v>
       </c>
       <c r="E6" s="17"/>
-      <c r="F6" s="31" t="s">
+      <c r="F6" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="G6" s="31" t="s">
+      <c r="G6" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="H6" s="31" t="s">
+      <c r="H6" s="30" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="37" t="s">
+      <c r="C7" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="37" t="s">
+      <c r="D7" s="36" t="s">
         <v>72</v>
       </c>
       <c r="E7" s="17"/>
-      <c r="F7" s="30" t="s">
+      <c r="F7" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="G7" s="30" t="s">
+      <c r="G7" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="H7" s="30" t="s">
+      <c r="H7" s="29" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="36" t="s">
+      <c r="A8" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="36" t="s">
+      <c r="D8" s="35" t="s">
         <v>71</v>
       </c>
       <c r="E8" s="17"/>
-      <c r="F8" s="31" t="s">
+      <c r="F8" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="G8" s="31" t="s">
+      <c r="G8" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="H8" s="31" t="s">
+      <c r="H8" s="30" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="C9" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="37" t="s">
+      <c r="D9" s="36" t="s">
         <v>73</v>
       </c>
       <c r="E9" s="17"/>
-      <c r="F9" s="32" t="s">
+      <c r="F9" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="G9" s="32" t="s">
+      <c r="G9" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="H9" s="32" t="s">
+      <c r="H9" s="31" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="36" t="s">
+      <c r="A10" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="C10" s="36" t="s">
+      <c r="C10" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="36" t="s">
+      <c r="D10" s="35" t="s">
         <v>76</v>
       </c>
       <c r="E10" s="17"/>
@@ -1732,122 +1949,122 @@
       <c r="H10" s="23"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="37" t="s">
+      <c r="A11" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="C11" s="37" t="s">
+      <c r="C11" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="37" t="s">
+      <c r="D11" s="36" t="s">
         <v>80</v>
       </c>
       <c r="E11" s="17"/>
-      <c r="F11" s="29" t="s">
+      <c r="F11" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G11" s="29" t="s">
+      <c r="G11" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="H11" s="29" t="s">
+      <c r="H11" s="28" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="36" t="s">
+      <c r="A12" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="C12" s="36" t="s">
+      <c r="C12" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="36" t="s">
+      <c r="D12" s="35" t="s">
         <v>77</v>
       </c>
       <c r="E12" s="17"/>
-      <c r="F12" s="30" t="s">
+      <c r="F12" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="G12" s="30" t="s">
+      <c r="G12" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="H12" s="30" t="s">
+      <c r="H12" s="29" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="37" t="s">
+      <c r="A13" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="B13" s="37" t="s">
+      <c r="B13" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="C13" s="37" t="s">
+      <c r="C13" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="37" t="s">
+      <c r="D13" s="36" t="s">
         <v>78</v>
       </c>
       <c r="E13" s="17"/>
-      <c r="F13" s="31" t="s">
+      <c r="F13" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="G13" s="31" t="s">
+      <c r="G13" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="H13" s="31" t="s">
+      <c r="H13" s="30" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="36" t="s">
+      <c r="A14" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="B14" s="36" t="s">
+      <c r="B14" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="C14" s="36" t="s">
+      <c r="C14" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="36" t="s">
+      <c r="D14" s="35" t="s">
         <v>79</v>
       </c>
       <c r="E14" s="17"/>
-      <c r="F14" s="30" t="s">
+      <c r="F14" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="G14" s="30" t="s">
+      <c r="G14" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="H14" s="30" t="s">
+      <c r="H14" s="29" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="37" t="s">
+      <c r="A15" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="C15" s="37" t="s">
+      <c r="C15" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="D15" s="37" t="s">
+      <c r="D15" s="36" t="s">
         <v>81</v>
       </c>
       <c r="E15" s="17"/>
-      <c r="F15" s="31" t="s">
+      <c r="F15" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="G15" s="31" t="s">
+      <c r="G15" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="H15" s="31" t="s">
+      <c r="H15" s="30" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1865,13 +2082,13 @@
         <v>82</v>
       </c>
       <c r="E16" s="17"/>
-      <c r="F16" s="32" t="s">
+      <c r="F16" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="G16" s="32" t="s">
+      <c r="G16" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="H16" s="32" t="s">
+      <c r="H16" s="31" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1890,22 +2107,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB50611C-C95E-47CD-8ED7-7DBE740143C6}">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.7109375" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" style="17" customWidth="1"/>
-    <col min="4" max="4" width="3.28515625" style="40" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" style="40" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" style="40" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" style="40" customWidth="1"/>
-    <col min="8" max="8" width="3" style="40" customWidth="1"/>
-    <col min="9" max="10" width="9.42578125" style="40" customWidth="1"/>
-    <col min="11" max="11" width="9.42578125" style="41" customWidth="1"/>
+    <col min="4" max="4" width="3.28515625" style="39" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" style="39" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" style="39" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" style="39" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3" style="39" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" style="39" customWidth="1"/>
+    <col min="10" max="10" width="24.7109375" style="39" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" style="40" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -1918,254 +2136,420 @@
       <c r="C1" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="E1" s="42" t="s">
+      <c r="E1" s="49" t="s">
         <v>141</v>
       </c>
-      <c r="F1" s="42" t="s">
+      <c r="F1" s="49" t="s">
         <v>143</v>
       </c>
-      <c r="G1" s="53" t="s">
+      <c r="G1" s="51" t="s">
         <v>142</v>
       </c>
-      <c r="K1" s="40"/>
+      <c r="I1" s="39" t="s">
+        <v>166</v>
+      </c>
+      <c r="J1" s="39" t="s">
+        <v>113</v>
+      </c>
+      <c r="K1" s="39"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="41" t="s">
         <v>120</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="C2" s="46" t="s">
+      <c r="C2" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
+      <c r="E2" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="F2" s="49" t="s">
+        <v>145</v>
+      </c>
+      <c r="G2" s="51" t="s">
+        <v>146</v>
+      </c>
+      <c r="I2" s="39" t="s">
+        <v>168</v>
+      </c>
+      <c r="J2" s="39" t="s">
+        <v>172</v>
+      </c>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="42" t="s">
         <v>121</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="C3" s="49" t="s">
+      <c r="C3" s="46" t="s">
         <v>125</v>
       </c>
-      <c r="K3" s="40"/>
-      <c r="L3" s="40"/>
-      <c r="M3" s="40"/>
+      <c r="E3" s="49" t="s">
+        <v>147</v>
+      </c>
+      <c r="F3" s="49" t="s">
+        <v>148</v>
+      </c>
+      <c r="G3" s="51" t="s">
+        <v>149</v>
+      </c>
+      <c r="I3" s="39" t="s">
+        <v>169</v>
+      </c>
+      <c r="J3" s="39" t="s">
+        <v>173</v>
+      </c>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="C4" s="44" t="s">
+      <c r="C4" s="41" t="s">
         <v>120</v>
       </c>
-      <c r="K4" s="40"/>
-      <c r="L4" s="40"/>
-      <c r="M4" s="40"/>
+      <c r="E4" s="49" t="s">
+        <v>150</v>
+      </c>
+      <c r="F4" s="49" t="s">
+        <v>151</v>
+      </c>
+      <c r="G4" s="49" t="s">
+        <v>152</v>
+      </c>
+      <c r="I4" s="50" t="s">
+        <v>170</v>
+      </c>
+      <c r="J4" s="39" t="s">
+        <v>174</v>
+      </c>
+      <c r="K4" s="39"/>
+      <c r="L4" s="39"/>
+      <c r="M4" s="39"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="47" t="s">
+      <c r="B5" s="17"/>
+      <c r="C5" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="K5" s="40"/>
-      <c r="L5" s="40"/>
-      <c r="M5" s="40"/>
+      <c r="E5" s="49" t="s">
+        <v>153</v>
+      </c>
+      <c r="F5" s="49" t="s">
+        <v>154</v>
+      </c>
+      <c r="G5" s="49" t="s">
+        <v>155</v>
+      </c>
+      <c r="I5" s="50" t="s">
+        <v>171</v>
+      </c>
+      <c r="J5" s="50" t="s">
+        <v>175</v>
+      </c>
+      <c r="K5" s="39"/>
+      <c r="L5" s="39"/>
+      <c r="M5" s="39"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="45" t="s">
         <v>124</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="48" t="s">
+      <c r="B6" s="17"/>
+      <c r="C6" s="45" t="s">
         <v>124</v>
       </c>
-      <c r="K6" s="40"/>
-      <c r="L6" s="40"/>
-      <c r="M6" s="40"/>
+      <c r="E6" s="49" t="s">
+        <v>156</v>
+      </c>
+      <c r="F6" s="49" t="s">
+        <v>157</v>
+      </c>
+      <c r="G6" s="49" t="s">
+        <v>158</v>
+      </c>
+      <c r="I6" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="J6" s="39" t="s">
+        <v>113</v>
+      </c>
+      <c r="K6" s="39"/>
+      <c r="L6" s="39"/>
+      <c r="M6" s="39"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="49" t="s">
+      <c r="A7" s="46" t="s">
         <v>125</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="C7" s="42" t="s">
         <v>121</v>
       </c>
-      <c r="K7" s="40"/>
-      <c r="L7" s="40"/>
-      <c r="M7" s="40"/>
+      <c r="E7" s="49" t="s">
+        <v>159</v>
+      </c>
+      <c r="F7" s="49" t="s">
+        <v>162</v>
+      </c>
+      <c r="G7" s="49" t="s">
+        <v>163</v>
+      </c>
+      <c r="I7" s="39" t="s">
+        <v>176</v>
+      </c>
+      <c r="J7" s="39" t="s">
+        <v>179</v>
+      </c>
+      <c r="K7" s="39"/>
+      <c r="L7" s="39"/>
+      <c r="M7" s="39"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="50" t="s">
+      <c r="A8" s="47" t="s">
         <v>126</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="50" t="s">
+      <c r="B8" s="17"/>
+      <c r="C8" s="47" t="s">
         <v>126</v>
       </c>
-      <c r="K8" s="40"/>
-      <c r="L8" s="40"/>
-      <c r="M8" s="40"/>
+      <c r="E8" s="49" t="s">
+        <v>160</v>
+      </c>
+      <c r="F8" s="49" t="s">
+        <v>163</v>
+      </c>
+      <c r="G8" s="49" t="s">
+        <v>162</v>
+      </c>
+      <c r="I8" s="39" t="s">
+        <v>177</v>
+      </c>
+      <c r="J8" s="39" t="s">
+        <v>180</v>
+      </c>
+      <c r="K8" s="39"/>
+      <c r="L8" s="39"/>
+      <c r="M8" s="39"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="51" t="s">
+      <c r="A9" s="48" t="s">
         <v>127</v>
       </c>
       <c r="B9" s="1"/>
-      <c r="C9" s="51" t="s">
+      <c r="C9" s="48" t="s">
         <v>127</v>
       </c>
-      <c r="K9" s="40"/>
-      <c r="L9" s="40"/>
-      <c r="M9" s="40"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K10" s="40"/>
-      <c r="L10" s="40"/>
-      <c r="M10" s="40"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="24" t="s">
+      <c r="E9" s="49" t="s">
+        <v>161</v>
+      </c>
+      <c r="F9" s="49" t="s">
+        <v>165</v>
+      </c>
+      <c r="G9" s="49" t="s">
+        <v>164</v>
+      </c>
+      <c r="I9" s="39" t="s">
+        <v>178</v>
+      </c>
+      <c r="J9" s="39" t="s">
+        <v>181</v>
+      </c>
+      <c r="K9" s="39"/>
+      <c r="L9" s="39"/>
+      <c r="M9" s="39"/>
+    </row>
+    <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K10" s="39"/>
+      <c r="L10" s="39"/>
+      <c r="M10" s="39"/>
+    </row>
+    <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="55" t="s">
         <v>130</v>
       </c>
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="61" t="s">
         <v>136</v>
       </c>
-      <c r="C11" s="43"/>
-      <c r="E11" t="s">
+      <c r="C11" s="61"/>
+      <c r="E11" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="61" t="s">
         <v>113</v>
       </c>
-      <c r="K11" s="40"/>
-      <c r="L11" s="40"/>
-      <c r="M11" s="40"/>
+      <c r="G11" s="61"/>
+      <c r="I11" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="J11" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="K11" s="39"/>
+      <c r="L11" s="39"/>
+      <c r="M11" s="39"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="56" t="s">
         <v>131</v>
       </c>
-      <c r="B12" s="43" t="s">
+      <c r="B12" s="62" t="s">
         <v>133</v>
       </c>
-      <c r="C12" s="43"/>
-      <c r="E12" t="s">
+      <c r="C12" s="62"/>
+      <c r="E12" s="60" t="s">
         <v>112</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="62" t="s">
         <v>117</v>
       </c>
-      <c r="K12" s="40"/>
-      <c r="L12" s="40"/>
-      <c r="M12" s="40"/>
+      <c r="G12" s="62"/>
+      <c r="I12" s="60" t="s">
+        <v>183</v>
+      </c>
+      <c r="J12" s="60" t="s">
+        <v>187</v>
+      </c>
+      <c r="K12" s="39"/>
+      <c r="L12" s="39"/>
+      <c r="M12" s="39"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="57" t="s">
         <v>137</v>
       </c>
-      <c r="B13" s="43" t="s">
+      <c r="B13" s="63" t="s">
         <v>132</v>
       </c>
-      <c r="C13" s="43"/>
-      <c r="E13" t="s">
+      <c r="C13" s="63"/>
+      <c r="E13" s="53" t="s">
         <v>108</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="63" t="s">
         <v>114</v>
       </c>
-      <c r="K13" s="40"/>
-      <c r="L13" s="40"/>
-      <c r="M13" s="40"/>
+      <c r="G13" s="63"/>
+      <c r="I13" s="66" t="s">
+        <v>184</v>
+      </c>
+      <c r="J13" s="66" t="s">
+        <v>188</v>
+      </c>
+      <c r="K13" s="39"/>
+      <c r="L13" s="39"/>
+      <c r="M13" s="39"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="58" t="s">
         <v>138</v>
       </c>
-      <c r="B14" s="43" t="s">
+      <c r="B14" s="64" t="s">
         <v>134</v>
       </c>
-      <c r="C14" s="43"/>
-      <c r="E14" t="s">
+      <c r="C14" s="64"/>
+      <c r="E14" s="52" t="s">
         <v>109</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="64" t="s">
         <v>115</v>
       </c>
-      <c r="K14" s="40"/>
-      <c r="L14" s="40"/>
-      <c r="M14" s="40"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="24" t="s">
+      <c r="G14" s="64"/>
+      <c r="I14" s="67" t="s">
+        <v>185</v>
+      </c>
+      <c r="J14" s="67" t="s">
+        <v>189</v>
+      </c>
+      <c r="K14" s="39"/>
+      <c r="L14" s="39"/>
+      <c r="M14" s="39"/>
+    </row>
+    <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="59" t="s">
         <v>139</v>
       </c>
-      <c r="B15" s="43" t="s">
+      <c r="B15" s="65" t="s">
         <v>135</v>
       </c>
-      <c r="C15" s="43"/>
-      <c r="E15" t="s">
+      <c r="C15" s="65"/>
+      <c r="E15" s="54" t="s">
         <v>110</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="65" t="s">
         <v>116</v>
       </c>
-      <c r="K15" s="40"/>
-      <c r="L15" s="40"/>
-      <c r="M15" s="40"/>
+      <c r="G15" s="65"/>
+      <c r="I15" s="54" t="s">
+        <v>186</v>
+      </c>
+      <c r="J15" s="54" t="s">
+        <v>190</v>
+      </c>
+      <c r="K15" s="39"/>
+      <c r="L15" s="39"/>
+      <c r="M15" s="39"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C16" s="52"/>
-      <c r="K16" s="40"/>
-      <c r="L16" s="40"/>
-      <c r="M16" s="40"/>
+      <c r="C16" s="49"/>
+      <c r="K16" s="39"/>
+      <c r="L16" s="39"/>
+      <c r="M16" s="39"/>
     </row>
     <row r="17" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C17" s="52"/>
-      <c r="K17" s="40"/>
+      <c r="C17" s="49"/>
+      <c r="K17" s="39"/>
     </row>
     <row r="18" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C18" s="52"/>
-      <c r="K18" s="40"/>
+      <c r="C18" s="49"/>
+      <c r="K18" s="39"/>
     </row>
     <row r="19" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C19" s="52"/>
+      <c r="C19" s="49"/>
     </row>
     <row r="20" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C20" s="52"/>
+      <c r="C20" s="49"/>
     </row>
     <row r="21" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C21" s="52"/>
+      <c r="C21" s="49"/>
     </row>
     <row r="22" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C22" s="52"/>
+      <c r="C22" s="49"/>
     </row>
     <row r="23" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C23" s="52"/>
+      <c r="C23" s="49"/>
     </row>
     <row r="24" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C24" s="52"/>
+      <c r="C24" s="49"/>
     </row>
     <row r="25" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C25" s="52"/>
+      <c r="C25" s="49"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="10">
     <mergeCell ref="B15:C15"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B13:C13"/>
@@ -2173,5 +2557,22 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <tableParts count="3">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70B7B516-DCFC-4AB6-BF06-408575EF620D}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
caracteristicas capa de enlace
</commit_message>
<xml_diff>
--- a/docs/protocols_suite.xlsx
+++ b/docs/protocols_suite.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\networks\CISCO\saves\ccna-s10\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EEE594A-D9DE-432E-AE77-DF2B0AEEF982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8A0CA88-CC85-4C3D-AE72-E343C70130D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="4" xr2:uid="{F2A32163-0D52-4F0A-8C5D-6317EB95D18F}"/>
+    <workbookView xWindow="30" yWindow="30" windowWidth="20460" windowHeight="10770" activeTab="3" xr2:uid="{F2A32163-0D52-4F0A-8C5D-6317EB95D18F}"/>
   </bookViews>
   <sheets>
     <sheet name="modelos" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="318">
   <si>
     <t>OSI de ISO</t>
   </si>
@@ -911,6 +911,90 @@
   </si>
   <si>
     <t>0x73</t>
+  </si>
+  <si>
+    <t>Tramas</t>
+  </si>
+  <si>
+    <t>RUNT</t>
+  </si>
+  <si>
+    <t>GIANT</t>
+  </si>
+  <si>
+    <t>CRC</t>
+  </si>
+  <si>
+    <t>THROTTLE</t>
+  </si>
+  <si>
+    <t>Descripcion</t>
+  </si>
+  <si>
+    <t>Tramas menores a 64B (Tamaño Min.)</t>
+  </si>
+  <si>
+    <t>Tramas mayores a 1,5KB (Tamaños Max.)</t>
+  </si>
+  <si>
+    <t>Error de Redundancia Ciclica (FCS)</t>
+  </si>
+  <si>
+    <t>Desbordamiendo de Buffer de Memoria</t>
+  </si>
+  <si>
+    <t>Fragment Free</t>
+  </si>
+  <si>
+    <t>Store &amp; Forward</t>
+  </si>
+  <si>
+    <t>Cut Through</t>
+  </si>
+  <si>
+    <t>Metodo</t>
+  </si>
+  <si>
+    <t>Reenvia la trama apenas recibe la misma</t>
+  </si>
+  <si>
+    <t>Almacena la trama y la reenvia despues de verificarla</t>
+  </si>
+  <si>
+    <t>Verifica los primero 64B antes de hacer el reenvio</t>
+  </si>
+  <si>
+    <t>Configuracion</t>
+  </si>
+  <si>
+    <t>SPEED</t>
+  </si>
+  <si>
+    <t>DUPLEX</t>
+  </si>
+  <si>
+    <t>MDIX</t>
+  </si>
+  <si>
+    <t>Establece en Ancho de Banda de la Interfaz</t>
+  </si>
+  <si>
+    <t>Define el tipo de comunicación del Enlace</t>
+  </si>
+  <si>
+    <t>Habilta la deteccion de Medios Cruzados</t>
+  </si>
+  <si>
+    <t>Ejemplo</t>
+  </si>
+  <si>
+    <t>speed 100</t>
+  </si>
+  <si>
+    <t>duplex half</t>
+  </si>
+  <si>
+    <t>mdix auto</t>
   </si>
 </sst>
 </file>
@@ -1067,7 +1151,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -1191,12 +1275,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1341,39 +1436,6 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1468,6 +1530,43 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1795,6 +1894,20 @@
 </table>
 </file>
 
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{136DDC96-ACB8-4F6A-B617-D837840061EF}" name="Tabla28" displayName="Tabla28" ref="E5:I7" totalsRowShown="0">
+  <autoFilter ref="E5:I7" xr:uid="{136DDC96-ACB8-4F6A-B617-D837840061EF}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{3F3BD8A5-519F-4E8C-B72E-94AF8EF2F6B9}" name="EXP"/>
+    <tableColumn id="2" xr3:uid="{406BD4BA-C7B8-475D-8C4D-353BAB801487}" name="16^3"/>
+    <tableColumn id="3" xr3:uid="{EE19687B-2AEB-4AB2-9B89-3560CB630422}" name="16^2"/>
+    <tableColumn id="4" xr3:uid="{0BEC878F-E44D-409F-A72D-A213B56B32DF}" name="16^1"/>
+    <tableColumn id="5" xr3:uid="{999D1ED4-B6FE-4D79-9FA2-75642F84B982}" name="16^0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{C78321D3-CCFD-43D7-8B50-0C45EEA5B1E7}" name="Tabla6" displayName="Tabla6" ref="I1:J5" totalsRowShown="0">
   <autoFilter ref="I1:J5" xr:uid="{C78321D3-CCFD-43D7-8B50-0C45EEA5B1E7}"/>
@@ -1818,6 +1931,40 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{1777475B-955E-4B5C-B1E4-7945829E45C1}" name="Tabla5" displayName="Tabla5" ref="A1:B5" totalsRowShown="0">
+  <autoFilter ref="A1:B5" xr:uid="{1777475B-955E-4B5C-B1E4-7945829E45C1}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{EA119109-3829-457F-9F4F-E397DEF4F4D7}" name="Tramas"/>
+    <tableColumn id="2" xr3:uid="{A8174C4F-8010-47E5-909A-590CB995DD81}" name="Descripcion"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{D7D4BAD5-9F16-44F0-B80D-BE151AB89E25}" name="Tabla9" displayName="Tabla9" ref="A7:B10" totalsRowShown="0">
+  <autoFilter ref="A7:B10" xr:uid="{D7D4BAD5-9F16-44F0-B80D-BE151AB89E25}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{46B1B41C-4BCA-44FC-9E28-E4E2B58EE4E2}" name="Metodo"/>
+    <tableColumn id="2" xr3:uid="{67AB0127-13A5-4D3C-A82C-2E5645C4DAC6}" name="Descripcion"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{D6E6288B-7C0A-44D4-A18C-AA07A1BBA539}" name="Tabla10" displayName="Tabla10" ref="D1:F4" totalsRowShown="0">
+  <autoFilter ref="D1:F4" xr:uid="{D6E6288B-7C0A-44D4-A18C-AA07A1BBA539}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{A315599C-C7E2-4B4E-BBA9-5E4AEA4F8A42}" name="Configuracion"/>
+    <tableColumn id="2" xr3:uid="{904F5868-24B9-4F90-AC10-9A94B67BACD8}" name="Descripcion"/>
+    <tableColumn id="3" xr3:uid="{29502F13-3442-4DE6-A562-AB650E8FCE95}" name="Ejemplo"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{42F81D43-1DF1-4805-95B1-B96C8A4790AB}" name="Tabla1" displayName="Tabla1" ref="A1:C21" totalsRowShown="0">
   <autoFilter ref="A1:C21" xr:uid="{42F81D43-1DF1-4805-95B1-B96C8A4790AB}"/>
   <tableColumns count="3">
@@ -1829,7 +1976,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3C826FE9-9026-4910-9978-0DF01EB75377}" name="Tabla2" displayName="Tabla2" ref="E1:I3" totalsRowShown="0">
   <autoFilter ref="E1:I3" xr:uid="{3C826FE9-9026-4910-9978-0DF01EB75377}"/>
   <tableColumns count="5">
@@ -1843,49 +1990,35 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E6370397-E076-43E7-9698-49F6F959CE7A}" name="Tabla25" displayName="Tabla25" ref="K1:S3" totalsRowShown="0">
   <autoFilter ref="K1:S3" xr:uid="{E6370397-E076-43E7-9698-49F6F959CE7A}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{D6A37B02-E9C4-49CB-8C2A-A865DDB05E2C}" name="EXP"/>
-    <tableColumn id="2" xr3:uid="{1349FDC6-3AA1-42B5-9F06-7FC58808E9C1}" name="2^7" dataDxfId="0">
+    <tableColumn id="2" xr3:uid="{1349FDC6-3AA1-42B5-9F06-7FC58808E9C1}" name="2^7" dataDxfId="7">
       <calculatedColumnFormula>2^7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{33EADDB5-4757-4423-BE0A-AB9102000FFB}" name="2^6" dataDxfId="1">
+    <tableColumn id="3" xr3:uid="{33EADDB5-4757-4423-BE0A-AB9102000FFB}" name="2^6" dataDxfId="6">
       <calculatedColumnFormula>2^6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{50E8A68B-6961-40D5-98D1-907DC09AFC45}" name="2^5" dataDxfId="2">
+    <tableColumn id="4" xr3:uid="{50E8A68B-6961-40D5-98D1-907DC09AFC45}" name="2^5" dataDxfId="5">
       <calculatedColumnFormula>2^5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C3D88FBD-0E0B-4446-8615-4D2D84ECB388}" name="2^4" dataDxfId="3">
+    <tableColumn id="5" xr3:uid="{C3D88FBD-0E0B-4446-8615-4D2D84ECB388}" name="2^4" dataDxfId="4">
       <calculatedColumnFormula>2^4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{34188D14-E91B-406C-A3AE-60F368E2A5FD}" name="2^3" dataDxfId="4">
+    <tableColumn id="6" xr3:uid="{34188D14-E91B-406C-A3AE-60F368E2A5FD}" name="2^3" dataDxfId="3">
       <calculatedColumnFormula>2^3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{109343F3-772B-401D-B6E1-CB46978A4E8A}" name="2^2" dataDxfId="5">
+    <tableColumn id="7" xr3:uid="{109343F3-772B-401D-B6E1-CB46978A4E8A}" name="2^2" dataDxfId="2">
       <calculatedColumnFormula>2^2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{4FEF6C42-FF4E-492F-9369-CB1247EAFFD2}" name="2^1" dataDxfId="6">
+    <tableColumn id="8" xr3:uid="{4FEF6C42-FF4E-492F-9369-CB1247EAFFD2}" name="2^1" dataDxfId="1">
       <calculatedColumnFormula>2^1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{8831B11E-9A44-40E1-A709-EAAB97E9E3BD}" name="2^0" dataDxfId="7">
+    <tableColumn id="9" xr3:uid="{8831B11E-9A44-40E1-A709-EAAB97E9E3BD}" name="2^0" dataDxfId="0">
       <calculatedColumnFormula>2^0</calculatedColumnFormula>
     </tableColumn>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{136DDC96-ACB8-4F6A-B617-D837840061EF}" name="Tabla28" displayName="Tabla28" ref="E5:I7" totalsRowShown="0">
-  <autoFilter ref="E5:I7" xr:uid="{136DDC96-ACB8-4F6A-B617-D837840061EF}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{3F3BD8A5-519F-4E8C-B72E-94AF8EF2F6B9}" name="EXP"/>
-    <tableColumn id="2" xr3:uid="{406BD4BA-C7B8-475D-8C4D-353BAB801487}" name="16^3"/>
-    <tableColumn id="3" xr3:uid="{EE19687B-2AEB-4AB2-9B89-3560CB630422}" name="16^2"/>
-    <tableColumn id="4" xr3:uid="{0BEC878F-E44D-409F-A72D-A213B56B32DF}" name="16^1"/>
-    <tableColumn id="5" xr3:uid="{999D1ED4-B6FE-4D79-9FA2-75642F84B982}" name="16^0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2221,13 +2354,13 @@
       <c r="A2" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="96" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="61" t="s">
+      <c r="C2" s="99" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="58" t="s">
+      <c r="D2" s="96" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2235,17 +2368,17 @@
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="59"/>
-      <c r="C3" s="62"/>
-      <c r="D3" s="59"/>
+      <c r="B3" s="97"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="97"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="59"/>
-      <c r="C4" s="62"/>
-      <c r="D4" s="59"/>
+      <c r="B4" s="97"/>
+      <c r="C4" s="100"/>
+      <c r="D4" s="97"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -2285,7 +2418,7 @@
       <c r="C7" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="60" t="s">
+      <c r="D7" s="98" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2299,7 +2432,7 @@
       <c r="C8" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="60"/>
+      <c r="D8" s="98"/>
     </row>
     <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
@@ -2364,16 +2497,16 @@
       <c r="J1" s="21"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="63" t="s">
+      <c r="A3" s="101" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="63"/>
-      <c r="C3" s="63"/>
-      <c r="F3" s="63" t="s">
+      <c r="B3" s="101"/>
+      <c r="C3" s="101"/>
+      <c r="F3" s="101" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
+      <c r="G3" s="101"/>
+      <c r="H3" s="101"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="27" t="s">
@@ -2533,11 +2666,11 @@
         <v>76</v>
       </c>
       <c r="E10" s="17"/>
-      <c r="F10" s="63" t="s">
+      <c r="F10" s="101" t="s">
         <v>95</v>
       </c>
-      <c r="G10" s="63"/>
-      <c r="H10" s="63"/>
+      <c r="G10" s="101"/>
+      <c r="H10" s="101"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="31" t="s">
@@ -2977,17 +3110,17 @@
       <c r="A11" s="50" t="s">
         <v>130</v>
       </c>
-      <c r="B11" s="65" t="s">
+      <c r="B11" s="103" t="s">
         <v>136</v>
       </c>
-      <c r="C11" s="65"/>
+      <c r="C11" s="103"/>
       <c r="E11" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="F11" s="65" t="s">
+      <c r="F11" s="103" t="s">
         <v>113</v>
       </c>
-      <c r="G11" s="65"/>
+      <c r="G11" s="103"/>
       <c r="I11" s="12" t="s">
         <v>182</v>
       </c>
@@ -3002,17 +3135,17 @@
       <c r="A12" s="51" t="s">
         <v>131</v>
       </c>
-      <c r="B12" s="66" t="s">
+      <c r="B12" s="104" t="s">
         <v>133</v>
       </c>
-      <c r="C12" s="66"/>
+      <c r="C12" s="104"/>
       <c r="E12" s="55" t="s">
         <v>112</v>
       </c>
-      <c r="F12" s="66" t="s">
+      <c r="F12" s="104" t="s">
         <v>117</v>
       </c>
-      <c r="G12" s="66"/>
+      <c r="G12" s="104"/>
       <c r="I12" s="55" t="s">
         <v>183</v>
       </c>
@@ -3027,17 +3160,17 @@
       <c r="A13" s="52" t="s">
         <v>137</v>
       </c>
-      <c r="B13" s="67" t="s">
+      <c r="B13" s="105" t="s">
         <v>132</v>
       </c>
-      <c r="C13" s="67"/>
+      <c r="C13" s="105"/>
       <c r="E13" s="48" t="s">
         <v>108</v>
       </c>
-      <c r="F13" s="67" t="s">
+      <c r="F13" s="105" t="s">
         <v>114</v>
       </c>
-      <c r="G13" s="67"/>
+      <c r="G13" s="105"/>
       <c r="I13" s="56" t="s">
         <v>184</v>
       </c>
@@ -3052,17 +3185,17 @@
       <c r="A14" s="53" t="s">
         <v>138</v>
       </c>
-      <c r="B14" s="68" t="s">
+      <c r="B14" s="106" t="s">
         <v>134</v>
       </c>
-      <c r="C14" s="68"/>
+      <c r="C14" s="106"/>
       <c r="E14" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="F14" s="68" t="s">
+      <c r="F14" s="106" t="s">
         <v>115</v>
       </c>
-      <c r="G14" s="68"/>
+      <c r="G14" s="106"/>
       <c r="I14" s="57" t="s">
         <v>185</v>
       </c>
@@ -3077,17 +3210,17 @@
       <c r="A15" s="54" t="s">
         <v>139</v>
       </c>
-      <c r="B15" s="64" t="s">
+      <c r="B15" s="102" t="s">
         <v>135</v>
       </c>
-      <c r="C15" s="64"/>
+      <c r="C15" s="102"/>
       <c r="E15" s="49" t="s">
         <v>110</v>
       </c>
-      <c r="F15" s="64" t="s">
+      <c r="F15" s="102" t="s">
         <v>116</v>
       </c>
-      <c r="G15" s="64"/>
+      <c r="G15" s="102"/>
       <c r="I15" s="49" t="s">
         <v>186</v>
       </c>
@@ -3158,13 +3291,136 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70B7B516-DCFC-4AB6-BF06-408575EF620D}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:F4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="39.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B1" t="s">
+        <v>295</v>
+      </c>
+      <c r="D1" t="s">
+        <v>307</v>
+      </c>
+      <c r="E1" t="s">
+        <v>295</v>
+      </c>
+      <c r="F1" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B2" t="s">
+        <v>296</v>
+      </c>
+      <c r="D2" t="s">
+        <v>308</v>
+      </c>
+      <c r="E2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F2" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>292</v>
+      </c>
+      <c r="B3" t="s">
+        <v>297</v>
+      </c>
+      <c r="D3" t="s">
+        <v>309</v>
+      </c>
+      <c r="E3" t="s">
+        <v>312</v>
+      </c>
+      <c r="F3" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B4" t="s">
+        <v>298</v>
+      </c>
+      <c r="D4" t="s">
+        <v>310</v>
+      </c>
+      <c r="E4" t="s">
+        <v>313</v>
+      </c>
+      <c r="F4" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>294</v>
+      </c>
+      <c r="B5" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>303</v>
+      </c>
+      <c r="B7" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>302</v>
+      </c>
+      <c r="B8" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>301</v>
+      </c>
+      <c r="B9" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>300</v>
+      </c>
+      <c r="B10" t="s">
+        <v>306</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="3">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -3172,16 +3428,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A54F4483-CBAC-4BEA-A628-30BC5CC8F957}">
   <dimension ref="A1:AC24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q13" sqref="Q13"/>
+      <selection pane="bottomLeft" activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9" style="69" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="70" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" style="69" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9" style="58" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="59" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" style="58" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="2.42578125" customWidth="1"/>
     <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
     <col min="6" max="9" width="6.140625" customWidth="1"/>
@@ -3194,13 +3450,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="58" t="s">
         <v>191</v>
       </c>
-      <c r="B1" s="70" t="s">
+      <c r="B1" s="59" t="s">
         <v>192</v>
       </c>
-      <c r="C1" s="69" t="s">
+      <c r="C1" s="58" t="s">
         <v>193</v>
       </c>
       <c r="E1" t="s">
@@ -3247,13 +3503,13 @@
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="58" t="s">
         <v>194</v>
       </c>
-      <c r="B2" s="70" t="s">
+      <c r="B2" s="59" t="s">
         <v>222</v>
       </c>
-      <c r="C2" s="69" t="s">
+      <c r="C2" s="58" t="s">
         <v>242</v>
       </c>
       <c r="E2" t="s">
@@ -3312,13 +3568,13 @@
       </c>
     </row>
     <row r="3" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="71" t="s">
+      <c r="A3" s="60" t="s">
         <v>195</v>
       </c>
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="61" t="s">
         <v>223</v>
       </c>
-      <c r="C3" s="71" t="s">
+      <c r="C3" s="60" t="s">
         <v>243</v>
       </c>
       <c r="E3" t="s">
@@ -3365,24 +3621,24 @@
       </c>
     </row>
     <row r="4" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="69" t="s">
+      <c r="A4" s="58" t="s">
         <v>196</v>
       </c>
-      <c r="B4" s="70" t="s">
+      <c r="B4" s="59" t="s">
         <v>224</v>
       </c>
-      <c r="C4" s="69" t="s">
+      <c r="C4" s="58" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="5" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="71" t="s">
+      <c r="A5" s="60" t="s">
         <v>197</v>
       </c>
-      <c r="B5" s="72" t="s">
+      <c r="B5" s="61" t="s">
         <v>225</v>
       </c>
-      <c r="C5" s="71" t="s">
+      <c r="C5" s="60" t="s">
         <v>245</v>
       </c>
       <c r="E5" t="s">
@@ -3403,7 +3659,7 @@
       <c r="K5" s="28" t="s">
         <v>191</v>
       </c>
-      <c r="L5" s="103" t="s">
+      <c r="L5" s="92" t="s">
         <v>195</v>
       </c>
       <c r="M5" s="28" t="s">
@@ -3415,7 +3671,7 @@
       <c r="O5" s="28" t="s">
         <v>198</v>
       </c>
-      <c r="P5" s="103" t="s">
+      <c r="P5" s="92" t="s">
         <v>199</v>
       </c>
       <c r="Q5" s="28" t="s">
@@ -3430,25 +3686,25 @@
       <c r="T5" s="28" t="s">
         <v>193</v>
       </c>
-      <c r="V5" s="63" t="s">
+      <c r="V5" s="101" t="s">
         <v>275</v>
       </c>
-      <c r="W5" s="63"/>
-      <c r="X5" s="63"/>
-      <c r="Y5" s="63"/>
-      <c r="Z5" s="63"/>
-      <c r="AA5" s="63"/>
-      <c r="AB5" s="63"/>
-      <c r="AC5" s="63"/>
+      <c r="W5" s="101"/>
+      <c r="X5" s="101"/>
+      <c r="Y5" s="101"/>
+      <c r="Z5" s="101"/>
+      <c r="AA5" s="101"/>
+      <c r="AB5" s="101"/>
+      <c r="AC5" s="101"/>
     </row>
     <row r="6" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="69" t="s">
+      <c r="A6" s="58" t="s">
         <v>198</v>
       </c>
-      <c r="B6" s="70" t="s">
+      <c r="B6" s="59" t="s">
         <v>226</v>
       </c>
-      <c r="C6" s="69" t="s">
+      <c r="C6" s="58" t="s">
         <v>246</v>
       </c>
       <c r="E6" t="s">
@@ -3470,57 +3726,57 @@
         <f>16^0</f>
         <v>1</v>
       </c>
-      <c r="K6" s="80">
+      <c r="K6" s="69">
         <v>32</v>
       </c>
-      <c r="L6" s="100">
-        <v>0</v>
-      </c>
-      <c r="M6" s="76">
-        <v>0</v>
-      </c>
-      <c r="N6" s="76">
-        <v>1</v>
-      </c>
-      <c r="O6" s="76">
-        <v>0</v>
-      </c>
-      <c r="P6" s="100">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="76">
-        <v>0</v>
-      </c>
-      <c r="R6" s="76">
-        <v>0</v>
-      </c>
-      <c r="S6" s="76">
-        <v>0</v>
-      </c>
-      <c r="T6" s="76" t="s">
+      <c r="L6" s="89">
+        <v>0</v>
+      </c>
+      <c r="M6" s="65">
+        <v>0</v>
+      </c>
+      <c r="N6" s="65">
+        <v>1</v>
+      </c>
+      <c r="O6" s="65">
+        <v>0</v>
+      </c>
+      <c r="P6" s="89">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="65">
+        <v>0</v>
+      </c>
+      <c r="R6" s="65">
+        <v>0</v>
+      </c>
+      <c r="S6" s="65">
+        <v>0</v>
+      </c>
+      <c r="T6" s="65" t="s">
         <v>277</v>
       </c>
       <c r="V6" s="18">
         <v>32</v>
       </c>
-      <c r="W6" s="84">
+      <c r="W6" s="73">
         <v>2</v>
       </c>
-      <c r="X6" s="75"/>
-      <c r="Y6" s="75"/>
-      <c r="Z6" s="75"/>
-      <c r="AA6" s="75"/>
-      <c r="AB6" s="91"/>
-      <c r="AC6" s="91"/>
+      <c r="X6" s="64"/>
+      <c r="Y6" s="64"/>
+      <c r="Z6" s="64"/>
+      <c r="AA6" s="64"/>
+      <c r="AB6" s="80"/>
+      <c r="AC6" s="80"/>
     </row>
     <row r="7" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="69" t="s">
+      <c r="A7" s="58" t="s">
         <v>199</v>
       </c>
-      <c r="B7" s="70" t="s">
+      <c r="B7" s="59" t="s">
         <v>227</v>
       </c>
-      <c r="C7" s="69" t="s">
+      <c r="C7" s="58" t="s">
         <v>247</v>
       </c>
       <c r="E7" t="s">
@@ -3538,180 +3794,180 @@
       <c r="I7" s="18">
         <v>9</v>
       </c>
-      <c r="K7" s="81">
+      <c r="K7" s="70">
         <v>127</v>
       </c>
-      <c r="L7" s="101">
-        <v>0</v>
-      </c>
-      <c r="M7" s="79">
-        <v>1</v>
-      </c>
-      <c r="N7" s="79">
-        <v>1</v>
-      </c>
-      <c r="O7" s="79">
-        <v>1</v>
-      </c>
-      <c r="P7" s="101">
-        <v>1</v>
-      </c>
-      <c r="Q7" s="77">
-        <v>1</v>
-      </c>
-      <c r="R7" s="77">
-        <v>1</v>
-      </c>
-      <c r="S7" s="77">
-        <v>1</v>
-      </c>
-      <c r="T7" s="79" t="s">
+      <c r="L7" s="90">
+        <v>0</v>
+      </c>
+      <c r="M7" s="68">
+        <v>1</v>
+      </c>
+      <c r="N7" s="68">
+        <v>1</v>
+      </c>
+      <c r="O7" s="68">
+        <v>1</v>
+      </c>
+      <c r="P7" s="90">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="66">
+        <v>1</v>
+      </c>
+      <c r="R7" s="66">
+        <v>1</v>
+      </c>
+      <c r="S7" s="66">
+        <v>1</v>
+      </c>
+      <c r="T7" s="68" t="s">
         <v>278</v>
       </c>
-      <c r="V7" s="87">
+      <c r="V7" s="76">
         <v>0</v>
       </c>
       <c r="W7" s="18">
         <v>16</v>
       </c>
-      <c r="X7" s="84">
+      <c r="X7" s="73">
         <v>2</v>
       </c>
-      <c r="Y7" s="75"/>
-      <c r="Z7" s="75"/>
-      <c r="AA7" s="75"/>
-      <c r="AB7" s="91"/>
-      <c r="AC7" s="91"/>
+      <c r="Y7" s="64"/>
+      <c r="Z7" s="64"/>
+      <c r="AA7" s="64"/>
+      <c r="AB7" s="80"/>
+      <c r="AC7" s="80"/>
     </row>
     <row r="8" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="69" t="s">
+      <c r="A8" s="58" t="s">
         <v>200</v>
       </c>
-      <c r="B8" s="70" t="s">
+      <c r="B8" s="59" t="s">
         <v>228</v>
       </c>
-      <c r="C8" s="69" t="s">
+      <c r="C8" s="58" t="s">
         <v>248</v>
       </c>
-      <c r="K8" s="82">
+      <c r="K8" s="71">
         <v>254</v>
       </c>
-      <c r="L8" s="102">
-        <v>1</v>
-      </c>
-      <c r="M8" s="99">
-        <v>1</v>
-      </c>
-      <c r="N8" s="99">
-        <v>1</v>
-      </c>
-      <c r="O8" s="99">
-        <v>1</v>
-      </c>
-      <c r="P8" s="102">
-        <v>1</v>
-      </c>
-      <c r="Q8" s="78">
-        <v>1</v>
-      </c>
-      <c r="R8" s="78">
-        <v>1</v>
-      </c>
-      <c r="S8" s="78">
-        <v>0</v>
-      </c>
-      <c r="T8" s="99" t="s">
+      <c r="L8" s="91">
+        <v>1</v>
+      </c>
+      <c r="M8" s="88">
+        <v>1</v>
+      </c>
+      <c r="N8" s="88">
+        <v>1</v>
+      </c>
+      <c r="O8" s="88">
+        <v>1</v>
+      </c>
+      <c r="P8" s="91">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="67">
+        <v>1</v>
+      </c>
+      <c r="R8" s="67">
+        <v>1</v>
+      </c>
+      <c r="S8" s="67">
+        <v>0</v>
+      </c>
+      <c r="T8" s="88" t="s">
         <v>279</v>
       </c>
       <c r="U8" s="35"/>
-      <c r="V8" s="97"/>
+      <c r="V8" s="86"/>
       <c r="W8" s="18">
         <v>0</v>
       </c>
       <c r="X8" s="18">
         <v>8</v>
       </c>
-      <c r="Y8" s="84">
+      <c r="Y8" s="73">
         <v>2</v>
       </c>
-      <c r="Z8" s="75"/>
-      <c r="AA8" s="75"/>
-      <c r="AB8" s="91"/>
-      <c r="AC8" s="91"/>
+      <c r="Z8" s="64"/>
+      <c r="AA8" s="64"/>
+      <c r="AB8" s="80"/>
+      <c r="AC8" s="80"/>
     </row>
     <row r="9" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="71" t="s">
+      <c r="A9" s="60" t="s">
         <v>201</v>
       </c>
-      <c r="B9" s="72" t="s">
+      <c r="B9" s="61" t="s">
         <v>229</v>
       </c>
-      <c r="C9" s="71" t="s">
+      <c r="C9" s="60" t="s">
         <v>249</v>
       </c>
       <c r="E9" s="18">
         <v>192</v>
       </c>
-      <c r="F9" s="18">
+      <c r="F9" s="108">
         <v>16</v>
       </c>
-      <c r="H9" s="63" t="s">
+      <c r="H9" s="101" t="s">
         <v>276</v>
       </c>
-      <c r="I9" s="63"/>
-      <c r="K9" s="81">
+      <c r="I9" s="101"/>
+      <c r="K9" s="70">
         <v>192</v>
       </c>
-      <c r="L9" s="101">
-        <v>1</v>
-      </c>
-      <c r="M9" s="79">
-        <v>1</v>
-      </c>
-      <c r="N9" s="79">
-        <v>0</v>
-      </c>
-      <c r="O9" s="79">
-        <v>0</v>
-      </c>
-      <c r="P9" s="101">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="77">
-        <v>0</v>
-      </c>
-      <c r="R9" s="77">
-        <v>0</v>
-      </c>
-      <c r="S9" s="77">
-        <v>0</v>
-      </c>
-      <c r="T9" s="79" t="s">
+      <c r="L9" s="90">
+        <v>1</v>
+      </c>
+      <c r="M9" s="68">
+        <v>1</v>
+      </c>
+      <c r="N9" s="68">
+        <v>0</v>
+      </c>
+      <c r="O9" s="68">
+        <v>0</v>
+      </c>
+      <c r="P9" s="90">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="66">
+        <v>0</v>
+      </c>
+      <c r="R9" s="66">
+        <v>0</v>
+      </c>
+      <c r="S9" s="66">
+        <v>0</v>
+      </c>
+      <c r="T9" s="68" t="s">
         <v>280</v>
       </c>
-      <c r="V9" s="90"/>
-      <c r="W9" s="96"/>
+      <c r="V9" s="79"/>
+      <c r="W9" s="85"/>
       <c r="X9" s="18">
         <v>0</v>
       </c>
       <c r="Y9" s="18">
         <v>4</v>
       </c>
-      <c r="Z9" s="84">
+      <c r="Z9" s="73">
         <v>2</v>
       </c>
-      <c r="AA9" s="75"/>
-      <c r="AB9" s="91"/>
-      <c r="AC9" s="91"/>
+      <c r="AA9" s="64"/>
+      <c r="AB9" s="80"/>
+      <c r="AC9" s="80"/>
     </row>
     <row r="10" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="69" t="s">
+      <c r="A10" s="58" t="s">
         <v>202</v>
       </c>
-      <c r="B10" s="70" t="s">
+      <c r="B10" s="59" t="s">
         <v>230</v>
       </c>
-      <c r="C10" s="69" t="s">
+      <c r="C10" s="58" t="s">
         <v>250</v>
       </c>
       <c r="E10" s="18">
@@ -3726,189 +3982,189 @@
       <c r="I10" s="18">
         <v>0</v>
       </c>
-      <c r="K10" s="82">
+      <c r="K10" s="71">
         <v>168</v>
       </c>
-      <c r="L10" s="102">
-        <v>1</v>
-      </c>
-      <c r="M10" s="99">
-        <v>0</v>
-      </c>
-      <c r="N10" s="99">
-        <v>1</v>
-      </c>
-      <c r="O10" s="99">
-        <v>0</v>
-      </c>
-      <c r="P10" s="102">
-        <v>1</v>
-      </c>
-      <c r="Q10" s="78">
-        <v>0</v>
-      </c>
-      <c r="R10" s="78">
-        <v>0</v>
-      </c>
-      <c r="S10" s="78">
-        <v>0</v>
-      </c>
-      <c r="T10" s="99" t="s">
+      <c r="L10" s="91">
+        <v>1</v>
+      </c>
+      <c r="M10" s="88">
+        <v>0</v>
+      </c>
+      <c r="N10" s="88">
+        <v>1</v>
+      </c>
+      <c r="O10" s="88">
+        <v>0</v>
+      </c>
+      <c r="P10" s="91">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="67">
+        <v>0</v>
+      </c>
+      <c r="R10" s="67">
+        <v>0</v>
+      </c>
+      <c r="S10" s="67">
+        <v>0</v>
+      </c>
+      <c r="T10" s="88" t="s">
         <v>281</v>
       </c>
       <c r="V10" s="18">
         <v>168</v>
       </c>
-      <c r="W10" s="92">
+      <c r="W10" s="81">
         <v>2</v>
       </c>
-      <c r="X10" s="96"/>
+      <c r="X10" s="85"/>
       <c r="Y10" s="18">
         <v>0</v>
       </c>
       <c r="Z10" s="18">
         <v>2</v>
       </c>
-      <c r="AA10" s="84">
+      <c r="AA10" s="73">
         <v>2</v>
       </c>
-      <c r="AB10" s="91"/>
-      <c r="AC10" s="91"/>
+      <c r="AB10" s="80"/>
+      <c r="AC10" s="80"/>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A11" s="69" t="s">
+      <c r="A11" s="58" t="s">
         <v>203</v>
       </c>
-      <c r="B11" s="70" t="s">
+      <c r="B11" s="59" t="s">
         <v>231</v>
       </c>
-      <c r="C11" s="69" t="s">
+      <c r="C11" s="58" t="s">
         <v>251</v>
       </c>
       <c r="E11" s="18"/>
       <c r="F11" s="18"/>
-      <c r="K11" s="81">
+      <c r="K11" s="70">
         <v>223</v>
       </c>
-      <c r="L11" s="101">
-        <v>1</v>
-      </c>
-      <c r="M11" s="79">
-        <v>1</v>
-      </c>
-      <c r="N11" s="79">
-        <v>0</v>
-      </c>
-      <c r="O11" s="79">
-        <v>1</v>
-      </c>
-      <c r="P11" s="101">
-        <v>1</v>
-      </c>
-      <c r="Q11" s="77">
-        <v>1</v>
-      </c>
-      <c r="R11" s="77">
-        <v>1</v>
-      </c>
-      <c r="S11" s="77">
-        <v>1</v>
-      </c>
-      <c r="T11" s="79" t="s">
+      <c r="L11" s="90">
+        <v>1</v>
+      </c>
+      <c r="M11" s="68">
+        <v>1</v>
+      </c>
+      <c r="N11" s="68">
+        <v>0</v>
+      </c>
+      <c r="O11" s="68">
+        <v>1</v>
+      </c>
+      <c r="P11" s="90">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="66">
+        <v>1</v>
+      </c>
+      <c r="R11" s="66">
+        <v>1</v>
+      </c>
+      <c r="S11" s="66">
+        <v>1</v>
+      </c>
+      <c r="T11" s="68" t="s">
         <v>282</v>
       </c>
-      <c r="V11" s="87">
+      <c r="V11" s="76">
         <v>0</v>
       </c>
       <c r="W11" s="18">
         <v>84</v>
       </c>
-      <c r="X11" s="92">
+      <c r="X11" s="81">
         <v>2</v>
       </c>
-      <c r="Y11" s="96"/>
+      <c r="Y11" s="85"/>
       <c r="Z11" s="18">
         <v>0</v>
       </c>
       <c r="AA11" s="18">
         <v>1</v>
       </c>
-      <c r="AB11" s="91"/>
-      <c r="AC11" s="91"/>
+      <c r="AB11" s="80"/>
+      <c r="AC11" s="80"/>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A12" s="69" t="s">
+      <c r="A12" s="58" t="s">
         <v>207</v>
       </c>
-      <c r="B12" s="70" t="s">
+      <c r="B12" s="59" t="s">
         <v>232</v>
       </c>
-      <c r="C12" s="69" t="s">
+      <c r="C12" s="58" t="s">
         <v>252</v>
       </c>
       <c r="E12" s="18">
         <v>56</v>
       </c>
-      <c r="F12" s="18">
+      <c r="F12" s="108">
         <v>16</v>
       </c>
       <c r="H12" t="s">
         <v>276</v>
       </c>
-      <c r="K12" s="82">
+      <c r="K12" s="71">
         <v>56</v>
       </c>
-      <c r="L12" s="102">
-        <v>0</v>
-      </c>
-      <c r="M12" s="99">
-        <v>0</v>
-      </c>
-      <c r="N12" s="99">
-        <v>1</v>
-      </c>
-      <c r="O12" s="99">
-        <v>1</v>
-      </c>
-      <c r="P12" s="102">
-        <v>1</v>
-      </c>
-      <c r="Q12" s="78">
-        <v>0</v>
-      </c>
-      <c r="R12" s="78">
-        <v>0</v>
-      </c>
-      <c r="S12" s="78">
-        <v>0</v>
-      </c>
-      <c r="T12" s="99" t="s">
+      <c r="L12" s="91">
+        <v>0</v>
+      </c>
+      <c r="M12" s="88">
+        <v>0</v>
+      </c>
+      <c r="N12" s="88">
+        <v>1</v>
+      </c>
+      <c r="O12" s="88">
+        <v>1</v>
+      </c>
+      <c r="P12" s="91">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="67">
+        <v>0</v>
+      </c>
+      <c r="R12" s="67">
+        <v>0</v>
+      </c>
+      <c r="S12" s="67">
+        <v>0</v>
+      </c>
+      <c r="T12" s="88" t="s">
         <v>283</v>
       </c>
       <c r="U12" s="35"/>
-      <c r="V12" s="89"/>
+      <c r="V12" s="78"/>
       <c r="W12" s="18">
         <v>0</v>
       </c>
       <c r="X12" s="18">
         <v>42</v>
       </c>
-      <c r="Y12" s="93">
+      <c r="Y12" s="82">
         <v>2</v>
       </c>
-      <c r="Z12" s="95"/>
-      <c r="AA12" s="98"/>
-      <c r="AB12" s="91"/>
-      <c r="AC12" s="91"/>
+      <c r="Z12" s="84"/>
+      <c r="AA12" s="87"/>
+      <c r="AB12" s="80"/>
+      <c r="AC12" s="80"/>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A13" s="69" t="s">
+      <c r="A13" s="58" t="s">
         <v>208</v>
       </c>
-      <c r="B13" s="70" t="s">
+      <c r="B13" s="59" t="s">
         <v>233</v>
       </c>
-      <c r="C13" s="69" t="s">
+      <c r="C13" s="58" t="s">
         <v>253</v>
       </c>
       <c r="E13" s="18">
@@ -3923,173 +4179,173 @@
       <c r="I13" s="18">
         <v>8</v>
       </c>
-      <c r="K13" s="81">
+      <c r="K13" s="70">
         <v>87</v>
       </c>
-      <c r="L13" s="101">
-        <v>0</v>
-      </c>
-      <c r="M13" s="79">
-        <v>1</v>
-      </c>
-      <c r="N13" s="79">
-        <v>0</v>
-      </c>
-      <c r="O13" s="79">
-        <v>1</v>
-      </c>
-      <c r="P13" s="101">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="77">
-        <v>1</v>
-      </c>
-      <c r="R13" s="77">
-        <v>1</v>
-      </c>
-      <c r="S13" s="77">
-        <v>1</v>
-      </c>
-      <c r="T13" s="79" t="s">
+      <c r="L13" s="90">
+        <v>0</v>
+      </c>
+      <c r="M13" s="68">
+        <v>1</v>
+      </c>
+      <c r="N13" s="68">
+        <v>0</v>
+      </c>
+      <c r="O13" s="68">
+        <v>1</v>
+      </c>
+      <c r="P13" s="90">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="66">
+        <v>1</v>
+      </c>
+      <c r="R13" s="66">
+        <v>1</v>
+      </c>
+      <c r="S13" s="66">
+        <v>1</v>
+      </c>
+      <c r="T13" s="68" t="s">
         <v>284</v>
       </c>
-      <c r="W13" s="86"/>
+      <c r="W13" s="75"/>
       <c r="X13" s="18">
         <v>0</v>
       </c>
-      <c r="Y13" s="88">
+      <c r="Y13" s="77">
         <v>21</v>
       </c>
-      <c r="Z13" s="94">
+      <c r="Z13" s="83">
         <v>2</v>
       </c>
-      <c r="AA13" s="91"/>
-      <c r="AB13" s="91"/>
-      <c r="AC13" s="91"/>
+      <c r="AA13" s="80"/>
+      <c r="AB13" s="80"/>
+      <c r="AC13" s="80"/>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A14" s="69" t="s">
+      <c r="A14" s="58" t="s">
         <v>209</v>
       </c>
-      <c r="B14" s="70" t="s">
+      <c r="B14" s="59" t="s">
         <v>234</v>
       </c>
-      <c r="C14" s="69" t="s">
+      <c r="C14" s="58" t="s">
         <v>254</v>
       </c>
-      <c r="K14" s="82">
+      <c r="K14" s="71">
         <v>130</v>
       </c>
-      <c r="L14" s="102">
-        <v>1</v>
-      </c>
-      <c r="M14" s="99">
-        <v>0</v>
-      </c>
-      <c r="N14" s="99">
-        <v>0</v>
-      </c>
-      <c r="O14" s="99">
-        <v>0</v>
-      </c>
-      <c r="P14" s="102">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="78">
-        <v>0</v>
-      </c>
-      <c r="R14" s="78">
-        <v>1</v>
-      </c>
-      <c r="S14" s="78">
-        <v>0</v>
-      </c>
-      <c r="T14" s="99" t="s">
+      <c r="L14" s="91">
+        <v>1</v>
+      </c>
+      <c r="M14" s="88">
+        <v>0</v>
+      </c>
+      <c r="N14" s="88">
+        <v>0</v>
+      </c>
+      <c r="O14" s="88">
+        <v>0</v>
+      </c>
+      <c r="P14" s="91">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="67">
+        <v>0</v>
+      </c>
+      <c r="R14" s="67">
+        <v>1</v>
+      </c>
+      <c r="S14" s="67">
+        <v>0</v>
+      </c>
+      <c r="T14" s="88" t="s">
         <v>285</v>
       </c>
-      <c r="X14" s="86"/>
-      <c r="Y14" s="88">
+      <c r="X14" s="75"/>
+      <c r="Y14" s="77">
         <v>1</v>
       </c>
       <c r="Z14">
         <v>10</v>
       </c>
-      <c r="AA14" s="94">
+      <c r="AA14" s="83">
         <v>2</v>
       </c>
-      <c r="AB14" s="91"/>
-      <c r="AC14" s="91"/>
+      <c r="AB14" s="80"/>
+      <c r="AC14" s="80"/>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A15" s="69" t="s">
+      <c r="A15" s="58" t="s">
         <v>210</v>
       </c>
-      <c r="B15" s="70" t="s">
+      <c r="B15" s="59" t="s">
         <v>235</v>
       </c>
-      <c r="C15" s="69" t="s">
+      <c r="C15" s="58" t="s">
         <v>255</v>
       </c>
       <c r="E15">
         <v>172</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="107">
         <v>16</v>
       </c>
-      <c r="H15" s="63" t="s">
+      <c r="H15" s="101" t="s">
         <v>276</v>
       </c>
-      <c r="I15" s="63"/>
-      <c r="K15" s="83">
+      <c r="I15" s="101"/>
+      <c r="K15" s="72">
         <v>172</v>
       </c>
-      <c r="L15" s="101">
-        <v>1</v>
-      </c>
-      <c r="M15" s="79">
-        <v>0</v>
-      </c>
-      <c r="N15" s="79">
-        <v>1</v>
-      </c>
-      <c r="O15" s="79">
-        <v>0</v>
-      </c>
-      <c r="P15" s="101">
-        <v>1</v>
-      </c>
-      <c r="Q15" s="79">
-        <v>1</v>
-      </c>
-      <c r="R15" s="79">
-        <v>0</v>
-      </c>
-      <c r="S15" s="79">
-        <v>0</v>
-      </c>
-      <c r="T15" s="79" t="s">
+      <c r="L15" s="90">
+        <v>1</v>
+      </c>
+      <c r="M15" s="68">
+        <v>0</v>
+      </c>
+      <c r="N15" s="68">
+        <v>1</v>
+      </c>
+      <c r="O15" s="68">
+        <v>0</v>
+      </c>
+      <c r="P15" s="90">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="68">
+        <v>1</v>
+      </c>
+      <c r="R15" s="68">
+        <v>0</v>
+      </c>
+      <c r="S15" s="68">
+        <v>0</v>
+      </c>
+      <c r="T15" s="68" t="s">
         <v>286</v>
       </c>
-      <c r="Y15" s="86"/>
+      <c r="Y15" s="75"/>
       <c r="Z15">
         <v>0</v>
       </c>
       <c r="AA15">
         <v>5</v>
       </c>
-      <c r="AB15" s="94">
+      <c r="AB15" s="83">
         <v>2</v>
       </c>
-      <c r="AC15" s="91"/>
+      <c r="AC15" s="80"/>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A16" s="69" t="s">
+      <c r="A16" s="58" t="s">
         <v>211</v>
       </c>
-      <c r="B16" s="70" t="s">
+      <c r="B16" s="59" t="s">
         <v>236</v>
       </c>
-      <c r="C16" s="69" t="s">
+      <c r="C16" s="58" t="s">
         <v>256</v>
       </c>
       <c r="E16">
@@ -4104,88 +4360,88 @@
       <c r="I16" s="18" t="s">
         <v>205</v>
       </c>
-      <c r="K16" s="82">
+      <c r="K16" s="71">
         <v>144</v>
       </c>
-      <c r="L16" s="102">
-        <v>1</v>
-      </c>
-      <c r="M16" s="99">
-        <v>0</v>
-      </c>
-      <c r="N16" s="99">
-        <v>0</v>
-      </c>
-      <c r="O16" s="99">
-        <v>1</v>
-      </c>
-      <c r="P16" s="102">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="78">
-        <v>0</v>
-      </c>
-      <c r="R16" s="78">
-        <v>0</v>
-      </c>
-      <c r="S16" s="78">
-        <v>0</v>
-      </c>
-      <c r="T16" s="99" t="s">
+      <c r="L16" s="91">
+        <v>1</v>
+      </c>
+      <c r="M16" s="88">
+        <v>0</v>
+      </c>
+      <c r="N16" s="88">
+        <v>0</v>
+      </c>
+      <c r="O16" s="88">
+        <v>1</v>
+      </c>
+      <c r="P16" s="91">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="67">
+        <v>0</v>
+      </c>
+      <c r="R16" s="67">
+        <v>0</v>
+      </c>
+      <c r="S16" s="67">
+        <v>0</v>
+      </c>
+      <c r="T16" s="88" t="s">
         <v>287</v>
       </c>
-      <c r="Z16" s="86"/>
+      <c r="Z16" s="75"/>
       <c r="AA16">
         <v>1</v>
       </c>
       <c r="AB16">
         <v>2</v>
       </c>
-      <c r="AC16" s="94">
+      <c r="AC16" s="83">
         <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="73" t="s">
+      <c r="A17" s="62" t="s">
         <v>212</v>
       </c>
-      <c r="B17" s="74" t="s">
+      <c r="B17" s="63" t="s">
         <v>221</v>
       </c>
-      <c r="C17" s="73" t="s">
+      <c r="C17" s="62" t="s">
         <v>257</v>
       </c>
-      <c r="K17" s="81">
+      <c r="K17" s="70">
         <v>237</v>
       </c>
-      <c r="L17" s="101">
-        <v>1</v>
-      </c>
-      <c r="M17" s="79">
-        <v>1</v>
-      </c>
-      <c r="N17" s="79">
-        <v>1</v>
-      </c>
-      <c r="O17" s="79">
-        <v>0</v>
-      </c>
-      <c r="P17" s="101">
-        <v>1</v>
-      </c>
-      <c r="Q17" s="77">
-        <v>1</v>
-      </c>
-      <c r="R17" s="77">
-        <v>0</v>
-      </c>
-      <c r="S17" s="77">
-        <v>1</v>
-      </c>
-      <c r="T17" s="79" t="s">
+      <c r="L17" s="90">
+        <v>1</v>
+      </c>
+      <c r="M17" s="68">
+        <v>1</v>
+      </c>
+      <c r="N17" s="68">
+        <v>1</v>
+      </c>
+      <c r="O17" s="68">
+        <v>0</v>
+      </c>
+      <c r="P17" s="90">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="66">
+        <v>1</v>
+      </c>
+      <c r="R17" s="66">
+        <v>0</v>
+      </c>
+      <c r="S17" s="66">
+        <v>1</v>
+      </c>
+      <c r="T17" s="68" t="s">
         <v>288</v>
       </c>
-      <c r="AA17" s="86"/>
+      <c r="AA17" s="75"/>
       <c r="AB17">
         <v>0</v>
       </c>
@@ -4194,168 +4450,174 @@
       </c>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A18" s="69" t="s">
+      <c r="A18" s="58" t="s">
         <v>213</v>
       </c>
-      <c r="B18" s="70" t="s">
+      <c r="B18" s="59" t="s">
         <v>220</v>
       </c>
-      <c r="C18" s="69" t="s">
+      <c r="C18" s="58" t="s">
         <v>238</v>
       </c>
-      <c r="K18" s="82">
+      <c r="K18" s="71">
         <v>115</v>
       </c>
-      <c r="L18" s="102">
-        <v>0</v>
-      </c>
-      <c r="M18" s="99">
-        <v>1</v>
-      </c>
-      <c r="N18" s="99">
-        <v>1</v>
-      </c>
-      <c r="O18" s="99">
-        <v>1</v>
-      </c>
-      <c r="P18" s="102">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="78">
-        <v>0</v>
-      </c>
-      <c r="R18" s="78">
-        <v>1</v>
-      </c>
-      <c r="S18" s="78">
-        <v>1</v>
-      </c>
-      <c r="T18" s="99" t="s">
+      <c r="L18" s="91">
+        <v>0</v>
+      </c>
+      <c r="M18" s="88">
+        <v>1</v>
+      </c>
+      <c r="N18" s="88">
+        <v>1</v>
+      </c>
+      <c r="O18" s="88">
+        <v>1</v>
+      </c>
+      <c r="P18" s="91">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="67">
+        <v>0</v>
+      </c>
+      <c r="R18" s="67">
+        <v>1</v>
+      </c>
+      <c r="S18" s="67">
+        <v>1</v>
+      </c>
+      <c r="T18" s="88" t="s">
         <v>289</v>
       </c>
-      <c r="AB18" s="86"/>
-      <c r="AC18" s="85"/>
+      <c r="AB18" s="75"/>
+      <c r="AC18" s="74"/>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A19" s="69" t="s">
+      <c r="A19" s="58" t="s">
         <v>214</v>
       </c>
-      <c r="B19" s="70" t="s">
+      <c r="B19" s="59" t="s">
         <v>219</v>
       </c>
-      <c r="C19" s="69" t="s">
+      <c r="C19" s="58" t="s">
         <v>239</v>
       </c>
-      <c r="K19" s="81">
+      <c r="K19" s="70">
         <v>216</v>
       </c>
-      <c r="L19" s="101"/>
-      <c r="M19" s="79"/>
-      <c r="N19" s="79"/>
-      <c r="O19" s="79"/>
-      <c r="P19" s="101"/>
-      <c r="Q19" s="77"/>
-      <c r="R19" s="77"/>
-      <c r="S19" s="77"/>
-      <c r="T19" s="79" t="s">
+      <c r="L19" s="90">
+        <v>1</v>
+      </c>
+      <c r="M19" s="68">
+        <v>1</v>
+      </c>
+      <c r="N19" s="68">
+        <v>0</v>
+      </c>
+      <c r="O19" s="68"/>
+      <c r="P19" s="90"/>
+      <c r="Q19" s="66"/>
+      <c r="R19" s="66"/>
+      <c r="S19" s="66"/>
+      <c r="T19" s="68" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A20" s="69" t="s">
+      <c r="A20" s="58" t="s">
         <v>215</v>
       </c>
-      <c r="B20" s="70" t="s">
+      <c r="B20" s="59" t="s">
         <v>218</v>
       </c>
-      <c r="C20" s="69" t="s">
+      <c r="C20" s="58" t="s">
         <v>240</v>
       </c>
-      <c r="K20" s="82">
+      <c r="K20" s="71">
         <v>81</v>
       </c>
-      <c r="L20" s="102"/>
-      <c r="M20" s="99"/>
-      <c r="N20" s="99"/>
-      <c r="O20" s="99"/>
-      <c r="P20" s="102"/>
-      <c r="Q20" s="78"/>
-      <c r="R20" s="78"/>
-      <c r="S20" s="78"/>
-      <c r="T20" s="99" t="s">
+      <c r="L20" s="91"/>
+      <c r="M20" s="88"/>
+      <c r="N20" s="88"/>
+      <c r="O20" s="88"/>
+      <c r="P20" s="91"/>
+      <c r="Q20" s="67"/>
+      <c r="R20" s="67"/>
+      <c r="S20" s="67"/>
+      <c r="T20" s="88" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A21" s="69" t="s">
+      <c r="A21" s="58" t="s">
         <v>216</v>
       </c>
-      <c r="B21" s="70" t="s">
+      <c r="B21" s="59" t="s">
         <v>217</v>
       </c>
-      <c r="C21" s="69" t="s">
+      <c r="C21" s="58" t="s">
         <v>241</v>
       </c>
-      <c r="K21" s="81">
+      <c r="K21" s="70">
         <v>22</v>
       </c>
-      <c r="L21" s="101"/>
-      <c r="M21" s="79"/>
-      <c r="N21" s="79"/>
-      <c r="O21" s="79"/>
-      <c r="P21" s="101"/>
-      <c r="Q21" s="77"/>
-      <c r="R21" s="77"/>
-      <c r="S21" s="77"/>
-      <c r="T21" s="79" t="s">
+      <c r="L21" s="90"/>
+      <c r="M21" s="68"/>
+      <c r="N21" s="68"/>
+      <c r="O21" s="68"/>
+      <c r="P21" s="90"/>
+      <c r="Q21" s="66"/>
+      <c r="R21" s="66"/>
+      <c r="S21" s="66"/>
+      <c r="T21" s="68" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="K22" s="82">
+      <c r="K22" s="71">
         <v>120</v>
       </c>
-      <c r="L22" s="102"/>
-      <c r="M22" s="99"/>
-      <c r="N22" s="99"/>
-      <c r="O22" s="99"/>
-      <c r="P22" s="102"/>
-      <c r="Q22" s="78"/>
-      <c r="R22" s="78"/>
-      <c r="S22" s="78"/>
-      <c r="T22" s="99" t="s">
+      <c r="L22" s="91"/>
+      <c r="M22" s="88"/>
+      <c r="N22" s="88"/>
+      <c r="O22" s="88"/>
+      <c r="P22" s="91"/>
+      <c r="Q22" s="67"/>
+      <c r="R22" s="67"/>
+      <c r="S22" s="67"/>
+      <c r="T22" s="88" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="K23" s="81">
+      <c r="K23" s="70">
         <v>230</v>
       </c>
-      <c r="L23" s="101"/>
-      <c r="M23" s="79"/>
-      <c r="N23" s="79"/>
-      <c r="O23" s="79"/>
-      <c r="P23" s="101"/>
-      <c r="Q23" s="77"/>
-      <c r="R23" s="77"/>
-      <c r="S23" s="77"/>
-      <c r="T23" s="79" t="s">
+      <c r="L23" s="90"/>
+      <c r="M23" s="68"/>
+      <c r="N23" s="68"/>
+      <c r="O23" s="68"/>
+      <c r="P23" s="90"/>
+      <c r="Q23" s="66"/>
+      <c r="R23" s="66"/>
+      <c r="S23" s="66"/>
+      <c r="T23" s="68" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="24" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K24" s="104">
+      <c r="K24" s="93">
         <v>195</v>
       </c>
-      <c r="L24" s="105"/>
-      <c r="M24" s="106"/>
-      <c r="N24" s="106"/>
-      <c r="O24" s="106"/>
-      <c r="P24" s="105"/>
-      <c r="Q24" s="106"/>
-      <c r="R24" s="106"/>
-      <c r="S24" s="106"/>
-      <c r="T24" s="106" t="s">
+      <c r="L24" s="94"/>
+      <c r="M24" s="95"/>
+      <c r="N24" s="95"/>
+      <c r="O24" s="95"/>
+      <c r="P24" s="94"/>
+      <c r="Q24" s="95"/>
+      <c r="R24" s="95"/>
+      <c r="S24" s="95"/>
+      <c r="T24" s="95" t="s">
         <v>237</v>
       </c>
     </row>

</xml_diff>

<commit_message>
clases de ip y operacion and
</commit_message>
<xml_diff>
--- a/docs/protocols_suite.xlsx
+++ b/docs/protocols_suite.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\networks\CISCO\saves\ccna-s10\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E304A37-62AC-49DB-AF25-52CA33B7A586}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{334B5F72-7FA3-4BD3-85AE-3D8FA1C5DFEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="30" windowWidth="20460" windowHeight="10770" activeTab="5" xr2:uid="{F2A32163-0D52-4F0A-8C5D-6317EB95D18F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="5" xr2:uid="{F2A32163-0D52-4F0A-8C5D-6317EB95D18F}"/>
   </bookViews>
   <sheets>
     <sheet name="modelos" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="404">
   <si>
     <t>OSI de ISO</t>
   </si>
@@ -1058,9 +1058,268 @@
     <t>240.0.0.0</t>
   </si>
   <si>
+    <t>11000000</t>
+  </si>
+  <si>
+    <t>10.0.0.0</t>
+  </si>
+  <si>
+    <t>172.16.0.0</t>
+  </si>
+  <si>
+    <t>172.31.255.255</t>
+  </si>
+  <si>
+    <t>192.168.0.0</t>
+  </si>
+  <si>
+    <t>Multicast</t>
+  </si>
+  <si>
+    <t>Research</t>
+  </si>
+  <si>
+    <t>10101100</t>
+  </si>
+  <si>
+    <t>10101100.
+00010000</t>
+  </si>
+  <si>
+    <t>10101100.
+00011111</t>
+  </si>
+  <si>
+    <t>11000000.
+10101000.
+00000000</t>
+  </si>
+  <si>
+    <t>11000000.
+10101000.
+11111111</t>
+  </si>
+  <si>
+    <t>Subnetting</t>
+  </si>
+  <si>
+    <t>CIDR</t>
+  </si>
+  <si>
+    <t>Hosts</t>
+  </si>
+  <si>
+    <t>Subnets</t>
+  </si>
+  <si>
+    <t>/8</t>
+  </si>
+  <si>
+    <t>/16</t>
+  </si>
+  <si>
+    <t>255.0.0.0</t>
+  </si>
+  <si>
+    <t>255.255.0.0</t>
+  </si>
+  <si>
+    <t>255.255.255.0</t>
+  </si>
+  <si>
+    <t>Mask</t>
+  </si>
+  <si>
+    <t>AND</t>
+  </si>
+  <si>
+    <t>IP</t>
+  </si>
+  <si>
+    <t>SM</t>
+  </si>
+  <si>
+    <t>NET</t>
+  </si>
+  <si>
+    <t>BC</t>
+  </si>
+  <si>
+    <t>BYTE 1</t>
+  </si>
+  <si>
+    <t>BYTE 2</t>
+  </si>
+  <si>
+    <t>BYTE 3</t>
+  </si>
+  <si>
+    <t>BYTE 4</t>
+  </si>
+  <si>
+    <t>10.54.232.25</t>
+  </si>
+  <si>
+    <t>172.19.125.30</t>
+  </si>
+  <si>
+    <t>192.168.33.14</t>
+  </si>
+  <si>
+    <t>00110110</t>
+  </si>
+  <si>
+    <t>11101000</t>
+  </si>
+  <si>
+    <t>00011001</t>
+  </si>
+  <si>
+    <r>
+      <t>0000</t>
+    </r>
     <r>
       <rPr>
         <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1111</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <t>00010011</t>
+  </si>
+  <si>
+    <t>01111101</t>
+  </si>
+  <si>
+    <t>00011110</t>
+  </si>
+  <si>
+    <t>172.19.0.0</t>
+  </si>
+  <si>
+    <t>172.19.255.255</t>
+  </si>
+  <si>
+    <t>10101000</t>
+  </si>
+  <si>
+    <t>00100001</t>
+  </si>
+  <si>
+    <t>192.168.33.0</t>
+  </si>
+  <si>
+    <t>192.168.33.255</t>
+  </si>
+  <si>
+    <t>172.21.47.0</t>
+  </si>
+  <si>
+    <t>00010101</t>
+  </si>
+  <si>
+    <t>00101111</t>
+  </si>
+  <si>
+    <t>172.21.0.0</t>
+  </si>
+  <si>
+    <t>172.21.255.255</t>
+  </si>
+  <si>
+    <t>192.168.255.31</t>
+  </si>
+  <si>
+    <t>192.168.255.0</t>
+  </si>
+  <si>
+    <t>00011111</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
         <color rgb="FFC00000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -1070,7 +1329,8 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
+        <b/>
+        <sz val="9"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -1081,7 +1341,8 @@
   <si>
     <r>
       <rPr>
-        <sz val="11"/>
+        <b/>
+        <sz val="9"/>
         <color rgb="FFC00000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -1091,7 +1352,8 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
+        <b/>
+        <sz val="9"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -1102,7 +1364,8 @@
   <si>
     <r>
       <rPr>
-        <sz val="11"/>
+        <b/>
+        <sz val="9"/>
         <color rgb="FFC00000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -1112,7 +1375,8 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
+        <b/>
+        <sz val="9"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -1123,7 +1387,8 @@
   <si>
     <r>
       <rPr>
-        <sz val="11"/>
+        <b/>
+        <sz val="9"/>
         <color rgb="FFC00000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -1133,7 +1398,8 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
+        <b/>
+        <sz val="9"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -1144,7 +1410,8 @@
   <si>
     <r>
       <rPr>
-        <sz val="11"/>
+        <b/>
+        <sz val="9"/>
         <color rgb="FFC00000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -1154,7 +1421,8 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
+        <b/>
+        <sz val="9"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -1165,7 +1433,8 @@
   <si>
     <r>
       <rPr>
-        <sz val="11"/>
+        <b/>
+        <sz val="9"/>
         <color rgb="FFC00000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -1175,7 +1444,8 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
+        <b/>
+        <sz val="9"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -1186,7 +1456,8 @@
   <si>
     <r>
       <rPr>
-        <sz val="11"/>
+        <b/>
+        <sz val="9"/>
         <color rgb="FFC00000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -1196,7 +1467,8 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
+        <b/>
+        <sz val="9"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -1207,7 +1479,31 @@
   <si>
     <r>
       <rPr>
-        <sz val="11"/>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1110</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1111</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
         <color rgb="FFC00000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -1217,7 +1513,8 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
+        <b/>
+        <sz val="9"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -1228,28 +1525,8 @@
   <si>
     <r>
       <rPr>
-        <sz val="11"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1110</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1111</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
+        <b/>
+        <sz val="9"/>
         <color rgb="FFC00000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -1259,82 +1536,14 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
+        <b/>
+        <sz val="9"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>1111</t>
     </r>
-  </si>
-  <si>
-    <t>10.0.0.0</t>
-  </si>
-  <si>
-    <t>172.16.0.0</t>
-  </si>
-  <si>
-    <t>172.31.255.255</t>
-  </si>
-  <si>
-    <t>192.168.0.0</t>
-  </si>
-  <si>
-    <t>Multicast</t>
-  </si>
-  <si>
-    <t>Research</t>
-  </si>
-  <si>
-    <t>10101100.
-00010000</t>
-  </si>
-  <si>
-    <t>10101100.
-00011111</t>
-  </si>
-  <si>
-    <t>11000000.
-10101000.
-00000000</t>
-  </si>
-  <si>
-    <t>11000000.
-10101000.
-11111111</t>
-  </si>
-  <si>
-    <t>Subnetting</t>
-  </si>
-  <si>
-    <t>CIDR</t>
-  </si>
-  <si>
-    <t>Hosts</t>
-  </si>
-  <si>
-    <t>Subnets</t>
-  </si>
-  <si>
-    <t>/8</t>
-  </si>
-  <si>
-    <t>/16</t>
-  </si>
-  <si>
-    <t>/24</t>
-  </si>
-  <si>
-    <t>255.0.0.0</t>
-  </si>
-  <si>
-    <t>255.255.0.0</t>
-  </si>
-  <si>
-    <t>255.255.255.0</t>
-  </si>
-  <si>
-    <t>Mask</t>
   </si>
 </sst>
 </file>
@@ -1345,7 +1554,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1389,6 +1598,36 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
       <color rgb="FFC00000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1504,7 +1743,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -1682,12 +1921,34 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1697,7 +1958,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="167">
+  <cellXfs count="214">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2004,17 +2265,14 @@
     <xf numFmtId="49" fontId="5" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2022,14 +2280,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2049,45 +2313,6 @@
     <xf numFmtId="49" fontId="1" fillId="9" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="10" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2100,50 +2325,227 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="7" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="10" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="7" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="10" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="10" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="10" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="10" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="10" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="10" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="10" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="10" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="10" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5316,60 +5718,60 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CFA7AEB-8644-4483-AADF-2BE5610CF495}">
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
+      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" style="111" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="111" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" style="112" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" style="113" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" style="112" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" style="113" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" style="111" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="111" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" style="112" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" style="113" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="112" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="113" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" style="114" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" style="113" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" style="113" customWidth="1"/>
     <col min="9" max="9" width="10" style="114" customWidth="1"/>
-    <col min="10" max="10" width="5.140625" style="110" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" style="110" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" style="110" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" style="110" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.140625" style="110" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.7109375" style="110" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10" style="110" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="129" t="s">
+      <c r="A1" s="130" t="s">
         <v>323</v>
       </c>
-      <c r="B1" s="130" t="s">
+      <c r="B1" s="131" t="s">
         <v>326</v>
       </c>
-      <c r="C1" s="131"/>
-      <c r="D1" s="131"/>
-      <c r="E1" s="132"/>
-      <c r="F1" s="148" t="s">
+      <c r="C1" s="132"/>
+      <c r="D1" s="132"/>
+      <c r="E1" s="133"/>
+      <c r="F1" s="136" t="s">
         <v>327</v>
       </c>
-      <c r="G1" s="149"/>
-      <c r="H1" s="149"/>
-      <c r="I1" s="150"/>
-      <c r="J1" s="128" t="s">
-        <v>358</v>
-      </c>
-      <c r="K1" s="128"/>
-      <c r="L1" s="128"/>
-      <c r="M1" s="128"/>
+      <c r="G1" s="137"/>
+      <c r="H1" s="137"/>
+      <c r="I1" s="138"/>
+      <c r="J1" s="198" t="s">
+        <v>350</v>
+      </c>
+      <c r="K1" s="199"/>
+      <c r="L1" s="199"/>
+      <c r="M1" s="200"/>
     </row>
     <row r="2" spans="1:13" s="115" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="50" t="s">
         <v>325</v>
       </c>
-      <c r="B2" s="133" t="s">
+      <c r="B2" s="134" t="s">
         <v>328</v>
       </c>
       <c r="C2" s="116" t="s">
@@ -5378,10 +5780,10 @@
       <c r="D2" s="117" t="s">
         <v>330</v>
       </c>
-      <c r="E2" s="134" t="s">
+      <c r="E2" s="135" t="s">
         <v>331</v>
       </c>
-      <c r="F2" s="151" t="s">
+      <c r="F2" s="139" t="s">
         <v>328</v>
       </c>
       <c r="G2" s="116" t="s">
@@ -5390,144 +5792,144 @@
       <c r="H2" s="117" t="s">
         <v>330</v>
       </c>
-      <c r="I2" s="134" t="s">
+      <c r="I2" s="135" t="s">
         <v>331</v>
       </c>
-      <c r="J2" s="118" t="s">
+      <c r="J2" s="201" t="s">
+        <v>351</v>
+      </c>
+      <c r="K2" s="118" t="s">
         <v>359</v>
       </c>
-      <c r="K2" s="118" t="s">
-        <v>368</v>
-      </c>
       <c r="L2" s="118" t="s">
-        <v>361</v>
-      </c>
-      <c r="M2" s="118" t="s">
-        <v>360</v>
+        <v>353</v>
+      </c>
+      <c r="M2" s="202" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="51" t="s">
         <v>204</v>
       </c>
-      <c r="B3" s="135" t="s">
+      <c r="B3" s="182" t="s">
         <v>333</v>
       </c>
-      <c r="C3" s="119" t="s">
-        <v>338</v>
-      </c>
-      <c r="D3" s="120">
+      <c r="C3" s="183" t="s">
+        <v>394</v>
+      </c>
+      <c r="D3" s="140">
         <v>127255255255</v>
       </c>
-      <c r="E3" s="136" t="s">
-        <v>339</v>
-      </c>
-      <c r="F3" s="152" t="s">
-        <v>348</v>
-      </c>
-      <c r="G3" s="121" t="s">
+      <c r="E3" s="184" t="s">
+        <v>395</v>
+      </c>
+      <c r="F3" s="172">
+        <v>1111111</v>
+      </c>
+      <c r="G3" s="173" t="s">
         <v>232</v>
       </c>
-      <c r="H3" s="120">
+      <c r="H3" s="140">
         <v>10255255255</v>
       </c>
-      <c r="I3" s="153" t="s">
+      <c r="I3" s="174" t="s">
         <v>232</v>
       </c>
-      <c r="J3" s="122" t="s">
-        <v>362</v>
-      </c>
-      <c r="K3" s="122" t="s">
-        <v>365</v>
-      </c>
-      <c r="L3" s="122">
-        <v>1</v>
-      </c>
-      <c r="M3" s="123">
+      <c r="J3" s="203" t="s">
+        <v>354</v>
+      </c>
+      <c r="K3" s="185" t="s">
+        <v>356</v>
+      </c>
+      <c r="L3" s="185">
+        <v>1</v>
+      </c>
+      <c r="M3" s="204">
         <f>2^24-2</f>
         <v>16777214</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="24" x14ac:dyDescent="0.25">
       <c r="A4" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="137" t="s">
+      <c r="B4" s="186" t="s">
         <v>334</v>
       </c>
-      <c r="C4" s="138" t="s">
+      <c r="C4" s="187" t="s">
+        <v>396</v>
+      </c>
+      <c r="D4" s="141">
+        <v>191255255255</v>
+      </c>
+      <c r="E4" s="188" t="s">
+        <v>397</v>
+      </c>
+      <c r="F4" s="175" t="s">
         <v>340</v>
       </c>
-      <c r="D4" s="139">
-        <v>191255255255</v>
-      </c>
-      <c r="E4" s="140" t="s">
+      <c r="G4" s="176" t="s">
+        <v>346</v>
+      </c>
+      <c r="H4" s="177" t="s">
         <v>341</v>
       </c>
-      <c r="F4" s="154" t="s">
-        <v>349</v>
-      </c>
-      <c r="G4" s="155" t="s">
-        <v>354</v>
-      </c>
-      <c r="H4" s="156" t="s">
-        <v>350</v>
-      </c>
-      <c r="I4" s="157" t="s">
+      <c r="I4" s="178" t="s">
+        <v>347</v>
+      </c>
+      <c r="J4" s="205" t="s">
         <v>355</v>
       </c>
-      <c r="J4" s="124" t="s">
-        <v>363</v>
-      </c>
-      <c r="K4" s="124" t="s">
-        <v>366</v>
-      </c>
-      <c r="L4" s="124">
+      <c r="K4" s="206" t="s">
+        <v>357</v>
+      </c>
+      <c r="L4" s="206">
         <v>16</v>
       </c>
-      <c r="M4" s="125">
+      <c r="M4" s="207">
         <f>2^16-2</f>
         <v>65534</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="36" x14ac:dyDescent="0.25">
       <c r="A5" s="53" t="s">
         <v>205</v>
       </c>
-      <c r="B5" s="141" t="s">
+      <c r="B5" s="189" t="s">
         <v>335</v>
       </c>
-      <c r="C5" s="142" t="s">
+      <c r="C5" s="190" t="s">
+        <v>398</v>
+      </c>
+      <c r="D5" s="142">
+        <v>223255255255</v>
+      </c>
+      <c r="E5" s="191" t="s">
+        <v>399</v>
+      </c>
+      <c r="F5" s="179" t="s">
         <v>342</v>
       </c>
-      <c r="D5" s="143">
-        <v>223255255255</v>
-      </c>
-      <c r="E5" s="144" t="s">
-        <v>343</v>
-      </c>
-      <c r="F5" s="158" t="s">
-        <v>351</v>
-      </c>
-      <c r="G5" s="159" t="s">
-        <v>356</v>
-      </c>
-      <c r="H5" s="143">
+      <c r="G5" s="180" t="s">
+        <v>348</v>
+      </c>
+      <c r="H5" s="142">
         <v>192168255255</v>
       </c>
-      <c r="I5" s="160" t="s">
-        <v>357</v>
-      </c>
-      <c r="J5" s="126" t="s">
-        <v>364</v>
-      </c>
-      <c r="K5" s="126" t="s">
-        <v>367</v>
-      </c>
-      <c r="L5" s="126">
+      <c r="I5" s="181" t="s">
+        <v>349</v>
+      </c>
+      <c r="J5" s="208" t="s">
+        <v>349</v>
+      </c>
+      <c r="K5" s="209" t="s">
+        <v>358</v>
+      </c>
+      <c r="L5" s="209">
         <v>256</v>
       </c>
-      <c r="M5" s="127">
+      <c r="M5" s="210">
         <f>2^8-2</f>
         <v>254</v>
       </c>
@@ -5536,84 +5938,616 @@
       <c r="A6" s="52" t="s">
         <v>324</v>
       </c>
-      <c r="B6" s="137" t="s">
+      <c r="B6" s="186" t="s">
         <v>336</v>
       </c>
-      <c r="C6" s="138" t="s">
-        <v>344</v>
-      </c>
-      <c r="D6" s="139">
+      <c r="C6" s="187" t="s">
+        <v>400</v>
+      </c>
+      <c r="D6" s="141">
         <v>239255255255</v>
       </c>
-      <c r="E6" s="140" t="s">
-        <v>346</v>
-      </c>
-      <c r="F6" s="161" t="s">
-        <v>352</v>
-      </c>
-      <c r="G6" s="162"/>
-      <c r="H6" s="162"/>
-      <c r="I6" s="163"/>
-      <c r="J6" s="124"/>
-      <c r="K6" s="124"/>
-      <c r="L6" s="124"/>
-      <c r="M6" s="124"/>
+      <c r="E6" s="188" t="s">
+        <v>401</v>
+      </c>
+      <c r="F6" s="192" t="s">
+        <v>343</v>
+      </c>
+      <c r="G6" s="193"/>
+      <c r="H6" s="193"/>
+      <c r="I6" s="194"/>
+      <c r="J6" s="192" t="s">
+        <v>343</v>
+      </c>
+      <c r="K6" s="193"/>
+      <c r="L6" s="193"/>
+      <c r="M6" s="194"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="53" t="s">
         <v>206</v>
       </c>
-      <c r="B7" s="141" t="s">
+      <c r="B7" s="189" t="s">
         <v>337</v>
       </c>
-      <c r="C7" s="142" t="s">
-        <v>345</v>
-      </c>
-      <c r="D7" s="143">
+      <c r="C7" s="190" t="s">
+        <v>402</v>
+      </c>
+      <c r="D7" s="142">
         <v>255255255255</v>
       </c>
-      <c r="E7" s="144" t="s">
-        <v>347</v>
-      </c>
-      <c r="F7" s="164" t="s">
-        <v>353</v>
-      </c>
-      <c r="G7" s="165"/>
-      <c r="H7" s="165"/>
-      <c r="I7" s="166"/>
-      <c r="J7" s="126"/>
-      <c r="K7" s="126"/>
-      <c r="L7" s="126"/>
-      <c r="M7" s="126"/>
+      <c r="E7" s="191" t="s">
+        <v>403</v>
+      </c>
+      <c r="F7" s="195" t="s">
+        <v>344</v>
+      </c>
+      <c r="G7" s="196"/>
+      <c r="H7" s="196"/>
+      <c r="I7" s="197"/>
+      <c r="J7" s="195" t="s">
+        <v>344</v>
+      </c>
+      <c r="K7" s="196"/>
+      <c r="L7" s="196"/>
+      <c r="M7" s="197"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="54" t="s">
         <v>332</v>
       </c>
-      <c r="B8" s="145">
+      <c r="B8" s="211">
         <f>2^32</f>
         <v>4294967296</v>
       </c>
-      <c r="C8" s="146"/>
-      <c r="D8" s="146"/>
-      <c r="E8" s="147"/>
-      <c r="F8" s="145">
+      <c r="C8" s="212"/>
+      <c r="D8" s="212"/>
+      <c r="E8" s="213"/>
+      <c r="F8" s="211">
         <f>2^32</f>
         <v>4294967296</v>
       </c>
-      <c r="G8" s="146"/>
-      <c r="H8" s="146"/>
-      <c r="I8" s="147"/>
-      <c r="J8" s="145">
+      <c r="G8" s="212"/>
+      <c r="H8" s="212"/>
+      <c r="I8" s="213"/>
+      <c r="J8" s="211">
         <f>2^32</f>
         <v>4294967296</v>
       </c>
-      <c r="K8" s="146"/>
-      <c r="L8" s="146"/>
-      <c r="M8" s="147"/>
+      <c r="K8" s="212"/>
+      <c r="L8" s="212"/>
+      <c r="M8" s="213"/>
+    </row>
+    <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="50" t="s">
+        <v>360</v>
+      </c>
+      <c r="B10" s="50" t="s">
+        <v>365</v>
+      </c>
+      <c r="C10" s="50" t="s">
+        <v>366</v>
+      </c>
+      <c r="D10" s="50" t="s">
+        <v>367</v>
+      </c>
+      <c r="E10" s="50" t="s">
+        <v>368</v>
+      </c>
+      <c r="F10" s="117" t="s">
+        <v>191</v>
+      </c>
+      <c r="G10" s="134" t="s">
+        <v>365</v>
+      </c>
+      <c r="H10" s="50" t="s">
+        <v>366</v>
+      </c>
+      <c r="I10" s="50" t="s">
+        <v>367</v>
+      </c>
+      <c r="J10" s="50" t="s">
+        <v>368</v>
+      </c>
+      <c r="K10" s="117" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="51" t="s">
+        <v>361</v>
+      </c>
+      <c r="B11" s="152" t="s">
+        <v>375</v>
+      </c>
+      <c r="C11" s="153" t="s">
+        <v>372</v>
+      </c>
+      <c r="D11" s="154" t="s">
+        <v>373</v>
+      </c>
+      <c r="E11" s="153" t="s">
+        <v>374</v>
+      </c>
+      <c r="F11" s="121" t="s">
+        <v>369</v>
+      </c>
+      <c r="G11" s="165" t="s">
+        <v>375</v>
+      </c>
+      <c r="H11" s="153" t="s">
+        <v>218</v>
+      </c>
+      <c r="I11" s="154" t="s">
+        <v>217</v>
+      </c>
+      <c r="J11" s="153" t="s">
+        <v>217</v>
+      </c>
+      <c r="K11" s="169">
+        <v>10100255255</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="52" t="s">
+        <v>362</v>
+      </c>
+      <c r="B12" s="155" t="s">
+        <v>376</v>
+      </c>
+      <c r="C12" s="156" t="s">
+        <v>222</v>
+      </c>
+      <c r="D12" s="157" t="s">
+        <v>222</v>
+      </c>
+      <c r="E12" s="156" t="s">
+        <v>222</v>
+      </c>
+      <c r="F12" s="123" t="s">
+        <v>356</v>
+      </c>
+      <c r="G12" s="166" t="s">
+        <v>376</v>
+      </c>
+      <c r="H12" s="156" t="s">
+        <v>222</v>
+      </c>
+      <c r="I12" s="157" t="s">
+        <v>222</v>
+      </c>
+      <c r="J12" s="156" t="s">
+        <v>222</v>
+      </c>
+      <c r="K12" s="124" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="53" t="s">
+        <v>363</v>
+      </c>
+      <c r="B13" s="158" t="s">
+        <v>232</v>
+      </c>
+      <c r="C13" s="159" t="s">
+        <v>222</v>
+      </c>
+      <c r="D13" s="160" t="s">
+        <v>222</v>
+      </c>
+      <c r="E13" s="159" t="s">
+        <v>222</v>
+      </c>
+      <c r="F13" s="126" t="s">
+        <v>339</v>
+      </c>
+      <c r="G13" s="167" t="s">
+        <v>232</v>
+      </c>
+      <c r="H13" s="159" t="s">
+        <v>222</v>
+      </c>
+      <c r="I13" s="160" t="s">
+        <v>222</v>
+      </c>
+      <c r="J13" s="159" t="s">
+        <v>222</v>
+      </c>
+      <c r="K13" s="127" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="54" t="s">
+        <v>364</v>
+      </c>
+      <c r="B14" s="161" t="s">
+        <v>232</v>
+      </c>
+      <c r="C14" s="162" t="s">
+        <v>217</v>
+      </c>
+      <c r="D14" s="163" t="s">
+        <v>217</v>
+      </c>
+      <c r="E14" s="162" t="s">
+        <v>217</v>
+      </c>
+      <c r="F14" s="164">
+        <v>10255255255</v>
+      </c>
+      <c r="G14" s="168" t="s">
+        <v>232</v>
+      </c>
+      <c r="H14" s="162" t="s">
+        <v>217</v>
+      </c>
+      <c r="I14" s="163" t="s">
+        <v>217</v>
+      </c>
+      <c r="J14" s="162" t="s">
+        <v>217</v>
+      </c>
+      <c r="K14" s="170">
+        <v>10255255255</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="50" t="s">
+        <v>360</v>
+      </c>
+      <c r="B16" s="50" t="s">
+        <v>365</v>
+      </c>
+      <c r="C16" s="50" t="s">
+        <v>366</v>
+      </c>
+      <c r="D16" s="50" t="s">
+        <v>367</v>
+      </c>
+      <c r="E16" s="50" t="s">
+        <v>368</v>
+      </c>
+      <c r="F16" s="117" t="s">
+        <v>191</v>
+      </c>
+      <c r="G16" s="134" t="s">
+        <v>365</v>
+      </c>
+      <c r="H16" s="50" t="s">
+        <v>366</v>
+      </c>
+      <c r="I16" s="50" t="s">
+        <v>367</v>
+      </c>
+      <c r="J16" s="50" t="s">
+        <v>368</v>
+      </c>
+      <c r="K16" s="117" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="51" t="s">
+        <v>361</v>
+      </c>
+      <c r="B17" s="146" t="s">
+        <v>345</v>
+      </c>
+      <c r="C17" s="119" t="s">
+        <v>377</v>
+      </c>
+      <c r="D17" s="120" t="s">
+        <v>378</v>
+      </c>
+      <c r="E17" s="119" t="s">
+        <v>379</v>
+      </c>
+      <c r="F17" s="143" t="s">
+        <v>370</v>
+      </c>
+      <c r="G17" s="165" t="s">
+        <v>345</v>
+      </c>
+      <c r="H17" s="153" t="s">
+        <v>387</v>
+      </c>
+      <c r="I17" s="154" t="s">
+        <v>388</v>
+      </c>
+      <c r="J17" s="153" t="s">
+        <v>222</v>
+      </c>
+      <c r="K17" s="169" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="52" t="s">
+        <v>362</v>
+      </c>
+      <c r="B18" s="147" t="s">
+        <v>217</v>
+      </c>
+      <c r="C18" s="112" t="s">
+        <v>217</v>
+      </c>
+      <c r="D18" s="148" t="s">
+        <v>222</v>
+      </c>
+      <c r="E18" s="112" t="s">
+        <v>222</v>
+      </c>
+      <c r="F18" s="122" t="s">
+        <v>357</v>
+      </c>
+      <c r="G18" s="166" t="s">
+        <v>217</v>
+      </c>
+      <c r="H18" s="156" t="s">
+        <v>217</v>
+      </c>
+      <c r="I18" s="157" t="s">
+        <v>222</v>
+      </c>
+      <c r="J18" s="156" t="s">
+        <v>222</v>
+      </c>
+      <c r="K18" s="124" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="53" t="s">
+        <v>363</v>
+      </c>
+      <c r="B19" s="149" t="s">
+        <v>345</v>
+      </c>
+      <c r="C19" s="125" t="s">
+        <v>377</v>
+      </c>
+      <c r="D19" s="150" t="s">
+        <v>222</v>
+      </c>
+      <c r="E19" s="125" t="s">
+        <v>222</v>
+      </c>
+      <c r="F19" s="144" t="s">
+        <v>380</v>
+      </c>
+      <c r="G19" s="167" t="s">
+        <v>345</v>
+      </c>
+      <c r="H19" s="159" t="s">
+        <v>387</v>
+      </c>
+      <c r="I19" s="160" t="s">
+        <v>222</v>
+      </c>
+      <c r="J19" s="159" t="s">
+        <v>222</v>
+      </c>
+      <c r="K19" s="127" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="54" t="s">
+        <v>364</v>
+      </c>
+      <c r="B20" s="151" t="s">
+        <v>345</v>
+      </c>
+      <c r="C20" s="145" t="s">
+        <v>377</v>
+      </c>
+      <c r="D20" s="163" t="s">
+        <v>217</v>
+      </c>
+      <c r="E20" s="162" t="s">
+        <v>217</v>
+      </c>
+      <c r="F20" s="128" t="s">
+        <v>381</v>
+      </c>
+      <c r="G20" s="168" t="s">
+        <v>345</v>
+      </c>
+      <c r="H20" s="162" t="s">
+        <v>387</v>
+      </c>
+      <c r="I20" s="163" t="s">
+        <v>217</v>
+      </c>
+      <c r="J20" s="162" t="s">
+        <v>217</v>
+      </c>
+      <c r="K20" s="170" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="50" t="s">
+        <v>360</v>
+      </c>
+      <c r="B22" s="50" t="s">
+        <v>365</v>
+      </c>
+      <c r="C22" s="50" t="s">
+        <v>366</v>
+      </c>
+      <c r="D22" s="50" t="s">
+        <v>367</v>
+      </c>
+      <c r="E22" s="50" t="s">
+        <v>368</v>
+      </c>
+      <c r="F22" s="117" t="s">
+        <v>191</v>
+      </c>
+      <c r="G22" s="50" t="s">
+        <v>365</v>
+      </c>
+      <c r="H22" s="50" t="s">
+        <v>366</v>
+      </c>
+      <c r="I22" s="50" t="s">
+        <v>367</v>
+      </c>
+      <c r="J22" s="50" t="s">
+        <v>368</v>
+      </c>
+      <c r="K22" s="117" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="51" t="s">
+        <v>361</v>
+      </c>
+      <c r="B23" s="146" t="s">
+        <v>338</v>
+      </c>
+      <c r="C23" s="119" t="s">
+        <v>382</v>
+      </c>
+      <c r="D23" s="120" t="s">
+        <v>383</v>
+      </c>
+      <c r="E23" s="119" t="s">
+        <v>236</v>
+      </c>
+      <c r="F23" s="143" t="s">
+        <v>371</v>
+      </c>
+      <c r="G23" s="146" t="s">
+        <v>338</v>
+      </c>
+      <c r="H23" s="119" t="s">
+        <v>382</v>
+      </c>
+      <c r="I23" s="120" t="s">
+        <v>217</v>
+      </c>
+      <c r="J23" s="119" t="s">
+        <v>393</v>
+      </c>
+      <c r="K23" s="143" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="52" t="s">
+        <v>362</v>
+      </c>
+      <c r="B24" s="147" t="s">
+        <v>217</v>
+      </c>
+      <c r="C24" s="112" t="s">
+        <v>217</v>
+      </c>
+      <c r="D24" s="148" t="s">
+        <v>217</v>
+      </c>
+      <c r="E24" s="112" t="s">
+        <v>222</v>
+      </c>
+      <c r="F24" s="122" t="s">
+        <v>358</v>
+      </c>
+      <c r="G24" s="147" t="s">
+        <v>217</v>
+      </c>
+      <c r="H24" s="112" t="s">
+        <v>217</v>
+      </c>
+      <c r="I24" s="148" t="s">
+        <v>217</v>
+      </c>
+      <c r="J24" s="112" t="s">
+        <v>222</v>
+      </c>
+      <c r="K24" s="122" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="53" t="s">
+        <v>363</v>
+      </c>
+      <c r="B25" s="149" t="s">
+        <v>338</v>
+      </c>
+      <c r="C25" s="125" t="s">
+        <v>382</v>
+      </c>
+      <c r="D25" s="150" t="s">
+        <v>383</v>
+      </c>
+      <c r="E25" s="125" t="s">
+        <v>222</v>
+      </c>
+      <c r="F25" s="144" t="s">
+        <v>384</v>
+      </c>
+      <c r="G25" s="149" t="s">
+        <v>338</v>
+      </c>
+      <c r="H25" s="125" t="s">
+        <v>382</v>
+      </c>
+      <c r="I25" s="150" t="s">
+        <v>217</v>
+      </c>
+      <c r="J25" s="125" t="s">
+        <v>222</v>
+      </c>
+      <c r="K25" s="144" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="54" t="s">
+        <v>364</v>
+      </c>
+      <c r="B26" s="151" t="s">
+        <v>338</v>
+      </c>
+      <c r="C26" s="145" t="s">
+        <v>382</v>
+      </c>
+      <c r="D26" s="129" t="s">
+        <v>383</v>
+      </c>
+      <c r="E26" s="145" t="s">
+        <v>217</v>
+      </c>
+      <c r="F26" s="128" t="s">
+        <v>385</v>
+      </c>
+      <c r="G26" s="151" t="s">
+        <v>338</v>
+      </c>
+      <c r="H26" s="145" t="s">
+        <v>382</v>
+      </c>
+      <c r="I26" s="129" t="s">
+        <v>217</v>
+      </c>
+      <c r="J26" s="145" t="s">
+        <v>217</v>
+      </c>
+      <c r="K26" s="171">
+        <v>192168255255</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="B8:E8"/>
@@ -5622,7 +6556,10 @@
     <mergeCell ref="J1:M1"/>
     <mergeCell ref="F8:I8"/>
     <mergeCell ref="J8:M8"/>
+    <mergeCell ref="J6:M6"/>
+    <mergeCell ref="J7:M7"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
protocolos y puertos capa de transporte
</commit_message>
<xml_diff>
--- a/docs/protocols_suite.xlsx
+++ b/docs/protocols_suite.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\networks\CISCO\saves\ccna-s10\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D94F498B-4AB1-48F3-A6FA-4BB4759D6C08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF82295-86FE-4DA8-8917-15C3F9AA4A31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="30" windowWidth="20460" windowHeight="10770" firstSheet="1" activeTab="9" xr2:uid="{F2A32163-0D52-4F0A-8C5D-6317EB95D18F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="10" xr2:uid="{F2A32163-0D52-4F0A-8C5D-6317EB95D18F}"/>
   </bookViews>
   <sheets>
     <sheet name="modelos" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="vlsm" sheetId="8" r:id="rId8"/>
     <sheet name="routing" sheetId="9" r:id="rId9"/>
     <sheet name="ipv6" sheetId="10" r:id="rId10"/>
+    <sheet name="transporte" sheetId="11" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">modelos!$C$1:$C$14</definedName>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1245" uniqueCount="756">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1273" uniqueCount="776">
   <si>
     <t>OSI de ISO</t>
   </si>
@@ -3526,6 +3527,69 @@
   </si>
   <si>
     <t>FE80::2E0:B0FF:F3BA:3BD7/64</t>
+  </si>
+  <si>
+    <t>TCP</t>
+  </si>
+  <si>
+    <t>UDP</t>
+  </si>
+  <si>
+    <t>Transport Control Protocol</t>
+  </si>
+  <si>
+    <t>User Datagram Protocol</t>
+  </si>
+  <si>
+    <t>Datagram</t>
+  </si>
+  <si>
+    <t>Confiable</t>
+  </si>
+  <si>
+    <t>Esfuerzo Max.</t>
+  </si>
+  <si>
+    <t>Funcion</t>
+  </si>
+  <si>
+    <t>identifica cada segmento para que puedan ser  reordenados al recibirse.</t>
+  </si>
+  <si>
+    <t>Reenvia los datagramas directamente a la capa de aplicación, como los recibe.</t>
+  </si>
+  <si>
+    <t>tftp - dhcp - dns</t>
+  </si>
+  <si>
+    <t>Puertos</t>
+  </si>
+  <si>
+    <t>Conocidos</t>
+  </si>
+  <si>
+    <t>Registrados</t>
+  </si>
+  <si>
+    <t>Dinamicos</t>
+  </si>
+  <si>
+    <t>http - https - ftp - sftp - pop3 - imap - smtp - ssh</t>
+  </si>
+  <si>
+    <t>WEBSOCKET
+ip:port
+31.13.94.35:443
+https://facebook.com</t>
+  </si>
+  <si>
+    <t>Cabecera</t>
+  </si>
+  <si>
+    <t>20B</t>
+  </si>
+  <si>
+    <t>8B</t>
   </si>
 </sst>
 </file>
@@ -3761,7 +3825,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -3991,12 +4055,65 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="305">
+  <cellXfs count="314">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4657,6 +4774,9 @@
     <xf numFmtId="49" fontId="5" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -4690,6 +4810,42 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="10" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="10" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="10" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4708,42 +4864,6 @@
     <xf numFmtId="0" fontId="1" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="10" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="10" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="10" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -4780,17 +4900,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -10237,6 +10381,30 @@
 </table>
 </file>
 
+<file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{46F0F7B6-6466-4004-803C-643CF3606774}" name="Tabla15" displayName="Tabla15" ref="A1:C7" totalsRowShown="0">
+  <autoFilter ref="A1:C7" xr:uid="{46F0F7B6-6466-4004-803C-643CF3606774}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{75393568-62DA-4C5D-96AD-E15CD91F7AD5}" name="Protocolos"/>
+    <tableColumn id="2" xr3:uid="{6BF45044-738D-4C96-9218-65FB2E08D23A}" name="TCP"/>
+    <tableColumn id="3" xr3:uid="{F0D2A917-DB56-49FF-A2FF-C80FA7607726}" name="UDP"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{D61A4807-FC9B-4EBA-9B1C-7252EA5B0D89}" name="Tabla21" displayName="Tabla21" ref="E1:G4" totalsRowShown="0">
+  <autoFilter ref="E1:G4" xr:uid="{D61A4807-FC9B-4EBA-9B1C-7252EA5B0D89}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{E7FCCE8F-1C63-46E0-8E3E-348AC722D9EB}" name="Puertos"/>
+    <tableColumn id="2" xr3:uid="{3DD61FE2-D062-44B6-929A-13B844E457C3}" name="INI"/>
+    <tableColumn id="3" xr3:uid="{012F97BF-F6C4-420A-B4E2-DBA36C31DCEF}" name="FIN"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{52135C1B-9F95-4015-B02C-B87CD34D509E}" name="Tabla8" displayName="Tabla8" ref="I6:J9" totalsRowShown="0">
   <autoFilter ref="I6:J9" xr:uid="{52135C1B-9F95-4015-B02C-B87CD34D509E}"/>
@@ -10641,8 +10809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26B8B09C-E1B7-4EAF-8A56-2848F2F39911}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C4"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10672,13 +10840,13 @@
       <c r="A2" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="260" t="s">
+      <c r="B2" s="261" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="263" t="s">
+      <c r="C2" s="264" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="260" t="s">
+      <c r="D2" s="261" t="s">
         <v>13</v>
       </c>
     </row>
@@ -10686,17 +10854,17 @@
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="261"/>
-      <c r="C3" s="264"/>
-      <c r="D3" s="261"/>
+      <c r="B3" s="262"/>
+      <c r="C3" s="265"/>
+      <c r="D3" s="262"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="261"/>
-      <c r="C4" s="264"/>
-      <c r="D4" s="261"/>
+      <c r="B4" s="262"/>
+      <c r="C4" s="265"/>
+      <c r="D4" s="262"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -10736,7 +10904,7 @@
       <c r="C7" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="262" t="s">
+      <c r="D7" s="263" t="s">
         <v>4</v>
       </c>
     </row>
@@ -10750,7 +10918,7 @@
       <c r="C8" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="262"/>
+      <c r="D8" s="263"/>
     </row>
     <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
@@ -10778,7 +10946,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7C472EF-3BB2-44C9-8C98-743821E0C5E8}">
   <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
@@ -10803,20 +10971,20 @@
       <c r="A1" s="220" t="s">
         <v>693</v>
       </c>
-      <c r="B1" s="303" t="s">
+      <c r="B1" s="302" t="s">
         <v>686</v>
       </c>
-      <c r="C1" s="303"/>
-      <c r="D1" s="303"/>
+      <c r="C1" s="302"/>
+      <c r="D1" s="302"/>
       <c r="E1" s="220" t="s">
         <v>685</v>
       </c>
-      <c r="F1" s="303" t="s">
+      <c r="F1" s="302" t="s">
         <v>684</v>
       </c>
-      <c r="G1" s="303"/>
-      <c r="H1" s="303"/>
-      <c r="I1" s="303"/>
+      <c r="G1" s="302"/>
+      <c r="H1" s="302"/>
+      <c r="I1" s="302"/>
       <c r="J1" s="220" t="s">
         <v>694</v>
       </c>
@@ -10990,17 +11158,17 @@
       <c r="A5" s="254" t="s">
         <v>679</v>
       </c>
-      <c r="B5" s="302" t="s">
+      <c r="B5" s="303" t="s">
         <v>695</v>
       </c>
-      <c r="C5" s="302"/>
-      <c r="D5" s="302"/>
-      <c r="E5" s="302"/>
-      <c r="F5" s="302"/>
-      <c r="G5" s="302"/>
-      <c r="H5" s="302"/>
-      <c r="I5" s="302"/>
-      <c r="J5" s="302"/>
+      <c r="C5" s="303"/>
+      <c r="D5" s="303"/>
+      <c r="E5" s="303"/>
+      <c r="F5" s="303"/>
+      <c r="G5" s="303"/>
+      <c r="H5" s="303"/>
+      <c r="I5" s="303"/>
+      <c r="J5" s="303"/>
       <c r="L5" s="145" t="s">
         <v>704</v>
       </c>
@@ -11028,33 +11196,33 @@
       <c r="A7" s="220" t="s">
         <v>718</v>
       </c>
-      <c r="B7" s="303" t="s">
+      <c r="B7" s="302" t="s">
         <v>719</v>
       </c>
-      <c r="C7" s="303"/>
-      <c r="D7" s="303"/>
-      <c r="E7" s="303"/>
-      <c r="F7" s="303"/>
-      <c r="G7" s="303"/>
-      <c r="H7" s="303"/>
-      <c r="I7" s="303"/>
-      <c r="J7" s="301"/>
+      <c r="C7" s="302"/>
+      <c r="D7" s="302"/>
+      <c r="E7" s="302"/>
+      <c r="F7" s="302"/>
+      <c r="G7" s="302"/>
+      <c r="H7" s="302"/>
+      <c r="I7" s="302"/>
+      <c r="J7" s="304"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="221" t="s">
         <v>736</v>
       </c>
-      <c r="B8" s="304" t="s">
+      <c r="B8" s="305" t="s">
         <v>732</v>
       </c>
-      <c r="C8" s="304"/>
-      <c r="D8" s="304"/>
-      <c r="E8" s="304"/>
-      <c r="F8" s="304"/>
-      <c r="G8" s="304"/>
-      <c r="H8" s="304"/>
-      <c r="I8" s="304"/>
-      <c r="J8" s="301"/>
+      <c r="C8" s="305"/>
+      <c r="D8" s="305"/>
+      <c r="E8" s="305"/>
+      <c r="F8" s="305"/>
+      <c r="G8" s="305"/>
+      <c r="H8" s="305"/>
+      <c r="I8" s="305"/>
+      <c r="J8" s="304"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="249" t="s">
@@ -11084,7 +11252,7 @@
       <c r="I9" s="139" t="s">
         <v>725</v>
       </c>
-      <c r="J9" s="301"/>
+      <c r="J9" s="304"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="250" t="s">
@@ -11114,55 +11282,55 @@
       <c r="I10" s="142" t="s">
         <v>725</v>
       </c>
-      <c r="J10" s="301"/>
+      <c r="J10" s="304"/>
     </row>
     <row r="11" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="254" t="s">
         <v>737</v>
       </c>
-      <c r="B11" s="302" t="s">
+      <c r="B11" s="303" t="s">
         <v>734</v>
       </c>
-      <c r="C11" s="302"/>
-      <c r="D11" s="302"/>
-      <c r="E11" s="302"/>
-      <c r="F11" s="302"/>
-      <c r="G11" s="302"/>
-      <c r="H11" s="302"/>
-      <c r="I11" s="302"/>
-      <c r="J11" s="301"/>
+      <c r="C11" s="303"/>
+      <c r="D11" s="303"/>
+      <c r="E11" s="303"/>
+      <c r="F11" s="303"/>
+      <c r="G11" s="303"/>
+      <c r="H11" s="303"/>
+      <c r="I11" s="303"/>
+      <c r="J11" s="304"/>
     </row>
     <row r="12" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="220" t="s">
         <v>718</v>
       </c>
-      <c r="B12" s="303" t="s">
+      <c r="B12" s="302" t="s">
         <v>719</v>
       </c>
-      <c r="C12" s="303"/>
-      <c r="D12" s="303"/>
-      <c r="E12" s="303"/>
-      <c r="F12" s="303"/>
-      <c r="G12" s="303"/>
-      <c r="H12" s="303"/>
-      <c r="I12" s="303"/>
-      <c r="J12" s="265"/>
+      <c r="C12" s="302"/>
+      <c r="D12" s="302"/>
+      <c r="E12" s="302"/>
+      <c r="F12" s="302"/>
+      <c r="G12" s="302"/>
+      <c r="H12" s="302"/>
+      <c r="I12" s="302"/>
+      <c r="J12" s="266"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="221" t="s">
         <v>736</v>
       </c>
-      <c r="B13" s="304" t="s">
+      <c r="B13" s="305" t="s">
         <v>735</v>
       </c>
-      <c r="C13" s="304"/>
-      <c r="D13" s="304"/>
-      <c r="E13" s="304"/>
-      <c r="F13" s="304"/>
-      <c r="G13" s="304"/>
-      <c r="H13" s="304"/>
-      <c r="I13" s="304"/>
-      <c r="J13" s="265"/>
+      <c r="C13" s="305"/>
+      <c r="D13" s="305"/>
+      <c r="E13" s="305"/>
+      <c r="F13" s="305"/>
+      <c r="G13" s="305"/>
+      <c r="H13" s="305"/>
+      <c r="I13" s="305"/>
+      <c r="J13" s="266"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="249" t="s">
@@ -11192,7 +11360,7 @@
       <c r="I14" s="139" t="s">
         <v>730</v>
       </c>
-      <c r="J14" s="265"/>
+      <c r="J14" s="266"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="250" t="s">
@@ -11222,55 +11390,55 @@
       <c r="I15" s="142" t="s">
         <v>730</v>
       </c>
-      <c r="J15" s="265"/>
+      <c r="J15" s="266"/>
     </row>
     <row r="16" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="254" t="s">
         <v>737</v>
       </c>
-      <c r="B16" s="302" t="s">
+      <c r="B16" s="303" t="s">
         <v>740</v>
       </c>
-      <c r="C16" s="302"/>
-      <c r="D16" s="302"/>
-      <c r="E16" s="302"/>
-      <c r="F16" s="302"/>
-      <c r="G16" s="302"/>
-      <c r="H16" s="302"/>
-      <c r="I16" s="302"/>
-      <c r="J16" s="265"/>
+      <c r="C16" s="303"/>
+      <c r="D16" s="303"/>
+      <c r="E16" s="303"/>
+      <c r="F16" s="303"/>
+      <c r="G16" s="303"/>
+      <c r="H16" s="303"/>
+      <c r="I16" s="303"/>
+      <c r="J16" s="266"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="220" t="s">
         <v>718</v>
       </c>
-      <c r="B17" s="303" t="s">
+      <c r="B17" s="302" t="s">
         <v>719</v>
       </c>
-      <c r="C17" s="303"/>
-      <c r="D17" s="303"/>
-      <c r="E17" s="303"/>
-      <c r="F17" s="303"/>
-      <c r="G17" s="303"/>
-      <c r="H17" s="303"/>
-      <c r="I17" s="303"/>
-      <c r="J17" s="265"/>
+      <c r="C17" s="302"/>
+      <c r="D17" s="302"/>
+      <c r="E17" s="302"/>
+      <c r="F17" s="302"/>
+      <c r="G17" s="302"/>
+      <c r="H17" s="302"/>
+      <c r="I17" s="302"/>
+      <c r="J17" s="266"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="221" t="s">
         <v>736</v>
       </c>
-      <c r="B18" s="304" t="s">
+      <c r="B18" s="305" t="s">
         <v>741</v>
       </c>
-      <c r="C18" s="304"/>
-      <c r="D18" s="304"/>
-      <c r="E18" s="304"/>
-      <c r="F18" s="304"/>
-      <c r="G18" s="304"/>
-      <c r="H18" s="304"/>
-      <c r="I18" s="304"/>
-      <c r="J18" s="265"/>
+      <c r="C18" s="305"/>
+      <c r="D18" s="305"/>
+      <c r="E18" s="305"/>
+      <c r="F18" s="305"/>
+      <c r="G18" s="305"/>
+      <c r="H18" s="305"/>
+      <c r="I18" s="305"/>
+      <c r="J18" s="266"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="249" t="s">
@@ -11300,7 +11468,7 @@
       <c r="I19" s="139" t="s">
         <v>746</v>
       </c>
-      <c r="J19" s="265"/>
+      <c r="J19" s="266"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="250" t="s">
@@ -11330,55 +11498,55 @@
       <c r="I20" s="142" t="s">
         <v>746</v>
       </c>
-      <c r="J20" s="265"/>
+      <c r="J20" s="266"/>
     </row>
     <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="254" t="s">
         <v>737</v>
       </c>
-      <c r="B21" s="302" t="s">
+      <c r="B21" s="303" t="s">
         <v>747</v>
       </c>
-      <c r="C21" s="302"/>
-      <c r="D21" s="302"/>
-      <c r="E21" s="302"/>
-      <c r="F21" s="302"/>
-      <c r="G21" s="302"/>
-      <c r="H21" s="302"/>
-      <c r="I21" s="302"/>
-      <c r="J21" s="265"/>
+      <c r="C21" s="303"/>
+      <c r="D21" s="303"/>
+      <c r="E21" s="303"/>
+      <c r="F21" s="303"/>
+      <c r="G21" s="303"/>
+      <c r="H21" s="303"/>
+      <c r="I21" s="303"/>
+      <c r="J21" s="266"/>
     </row>
     <row r="22" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="220" t="s">
         <v>718</v>
       </c>
-      <c r="B22" s="303" t="s">
+      <c r="B22" s="302" t="s">
         <v>719</v>
       </c>
-      <c r="C22" s="303"/>
-      <c r="D22" s="303"/>
-      <c r="E22" s="303"/>
-      <c r="F22" s="303"/>
-      <c r="G22" s="303"/>
-      <c r="H22" s="303"/>
-      <c r="I22" s="303"/>
-      <c r="J22" s="265"/>
+      <c r="C22" s="302"/>
+      <c r="D22" s="302"/>
+      <c r="E22" s="302"/>
+      <c r="F22" s="302"/>
+      <c r="G22" s="302"/>
+      <c r="H22" s="302"/>
+      <c r="I22" s="302"/>
+      <c r="J22" s="266"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="221" t="s">
         <v>736</v>
       </c>
-      <c r="B23" s="304" t="s">
+      <c r="B23" s="305" t="s">
         <v>748</v>
       </c>
-      <c r="C23" s="304"/>
-      <c r="D23" s="304"/>
-      <c r="E23" s="304"/>
-      <c r="F23" s="304"/>
-      <c r="G23" s="304"/>
-      <c r="H23" s="304"/>
-      <c r="I23" s="304"/>
-      <c r="J23" s="265"/>
+      <c r="C23" s="305"/>
+      <c r="D23" s="305"/>
+      <c r="E23" s="305"/>
+      <c r="F23" s="305"/>
+      <c r="G23" s="305"/>
+      <c r="H23" s="305"/>
+      <c r="I23" s="305"/>
+      <c r="J23" s="266"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="249" t="s">
@@ -11408,7 +11576,7 @@
       <c r="I24" s="139" t="s">
         <v>754</v>
       </c>
-      <c r="J24" s="265"/>
+      <c r="J24" s="266"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="250" t="s">
@@ -11438,31 +11606,26 @@
       <c r="I25" s="142" t="s">
         <v>754</v>
       </c>
-      <c r="J25" s="265"/>
+      <c r="J25" s="266"/>
     </row>
     <row r="26" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="254" t="s">
         <v>737</v>
       </c>
-      <c r="B26" s="302" t="s">
+      <c r="B26" s="303" t="s">
         <v>755</v>
       </c>
-      <c r="C26" s="302"/>
-      <c r="D26" s="302"/>
-      <c r="E26" s="302"/>
-      <c r="F26" s="302"/>
-      <c r="G26" s="302"/>
-      <c r="H26" s="302"/>
-      <c r="I26" s="302"/>
-      <c r="J26" s="265"/>
+      <c r="C26" s="303"/>
+      <c r="D26" s="303"/>
+      <c r="E26" s="303"/>
+      <c r="F26" s="303"/>
+      <c r="G26" s="303"/>
+      <c r="H26" s="303"/>
+      <c r="I26" s="303"/>
+      <c r="J26" s="266"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="B5:J5"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="J7:J11"/>
     <mergeCell ref="J12:J16"/>
     <mergeCell ref="J17:J21"/>
     <mergeCell ref="J22:J26"/>
@@ -11470,17 +11633,173 @@
     <mergeCell ref="B12:I12"/>
     <mergeCell ref="B17:I17"/>
     <mergeCell ref="B22:I22"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B11:I11"/>
     <mergeCell ref="B13:I13"/>
     <mergeCell ref="B16:I16"/>
     <mergeCell ref="B18:I18"/>
     <mergeCell ref="B23:I23"/>
     <mergeCell ref="B21:I21"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="B5:J5"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="J7:J11"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B11:I11"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E77F6C1-0806-4014-AD32-965CFE63ECC4}">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="23.7109375" customWidth="1"/>
+    <col min="4" max="4" width="2.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="6.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>756</v>
+      </c>
+      <c r="C1" t="s">
+        <v>757</v>
+      </c>
+      <c r="E1" t="s">
+        <v>767</v>
+      </c>
+      <c r="F1" t="s">
+        <v>697</v>
+      </c>
+      <c r="G1" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" t="s">
+        <v>758</v>
+      </c>
+      <c r="C2" t="s">
+        <v>759</v>
+      </c>
+      <c r="E2" t="s">
+        <v>768</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>760</v>
+      </c>
+      <c r="E3" t="s">
+        <v>769</v>
+      </c>
+      <c r="F3">
+        <v>1024</v>
+      </c>
+      <c r="G3">
+        <v>49151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>773</v>
+      </c>
+      <c r="B4" t="s">
+        <v>774</v>
+      </c>
+      <c r="C4" t="s">
+        <v>775</v>
+      </c>
+      <c r="E4" t="s">
+        <v>770</v>
+      </c>
+      <c r="F4">
+        <v>49152</v>
+      </c>
+      <c r="G4">
+        <v>65535</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" t="s">
+        <v>761</v>
+      </c>
+      <c r="C5" t="s">
+        <v>762</v>
+      </c>
+      <c r="F5" s="307"/>
+      <c r="G5" s="307"/>
+    </row>
+    <row r="6" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="103" t="s">
+        <v>763</v>
+      </c>
+      <c r="B6" s="306" t="s">
+        <v>764</v>
+      </c>
+      <c r="C6" s="306" t="s">
+        <v>765</v>
+      </c>
+      <c r="E6" s="308" t="s">
+        <v>772</v>
+      </c>
+      <c r="F6" s="309"/>
+      <c r="G6" s="310"/>
+    </row>
+    <row r="7" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="103" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="260" t="s">
+        <v>771</v>
+      </c>
+      <c r="C7" s="103" t="s">
+        <v>766</v>
+      </c>
+      <c r="E7" s="311"/>
+      <c r="F7" s="312"/>
+      <c r="G7" s="313"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E6:G7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -11525,16 +11844,16 @@
       <c r="J1" s="21"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="265" t="s">
+      <c r="A3" s="266" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="265"/>
-      <c r="C3" s="265"/>
-      <c r="F3" s="265" t="s">
+      <c r="B3" s="266"/>
+      <c r="C3" s="266"/>
+      <c r="F3" s="266" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="265"/>
-      <c r="H3" s="265"/>
+      <c r="G3" s="266"/>
+      <c r="H3" s="266"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="27" t="s">
@@ -11694,11 +12013,11 @@
         <v>76</v>
       </c>
       <c r="E10" s="17"/>
-      <c r="F10" s="265" t="s">
+      <c r="F10" s="266" t="s">
         <v>95</v>
       </c>
-      <c r="G10" s="265"/>
-      <c r="H10" s="265"/>
+      <c r="G10" s="266"/>
+      <c r="H10" s="266"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="31" t="s">
@@ -12138,17 +12457,17 @@
       <c r="A11" s="50" t="s">
         <v>130</v>
       </c>
-      <c r="B11" s="267" t="s">
+      <c r="B11" s="268" t="s">
         <v>136</v>
       </c>
-      <c r="C11" s="267"/>
+      <c r="C11" s="268"/>
       <c r="E11" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="F11" s="267" t="s">
+      <c r="F11" s="268" t="s">
         <v>113</v>
       </c>
-      <c r="G11" s="267"/>
+      <c r="G11" s="268"/>
       <c r="I11" s="12" t="s">
         <v>182</v>
       </c>
@@ -12163,17 +12482,17 @@
       <c r="A12" s="51" t="s">
         <v>131</v>
       </c>
-      <c r="B12" s="268" t="s">
+      <c r="B12" s="269" t="s">
         <v>133</v>
       </c>
-      <c r="C12" s="268"/>
+      <c r="C12" s="269"/>
       <c r="E12" s="55" t="s">
         <v>112</v>
       </c>
-      <c r="F12" s="268" t="s">
+      <c r="F12" s="269" t="s">
         <v>117</v>
       </c>
-      <c r="G12" s="268"/>
+      <c r="G12" s="269"/>
       <c r="I12" s="55" t="s">
         <v>183</v>
       </c>
@@ -12188,17 +12507,17 @@
       <c r="A13" s="52" t="s">
         <v>137</v>
       </c>
-      <c r="B13" s="269" t="s">
+      <c r="B13" s="270" t="s">
         <v>132</v>
       </c>
-      <c r="C13" s="269"/>
+      <c r="C13" s="270"/>
       <c r="E13" s="48" t="s">
         <v>108</v>
       </c>
-      <c r="F13" s="269" t="s">
+      <c r="F13" s="270" t="s">
         <v>114</v>
       </c>
-      <c r="G13" s="269"/>
+      <c r="G13" s="270"/>
       <c r="I13" s="56" t="s">
         <v>184</v>
       </c>
@@ -12213,17 +12532,17 @@
       <c r="A14" s="53" t="s">
         <v>138</v>
       </c>
-      <c r="B14" s="270" t="s">
+      <c r="B14" s="271" t="s">
         <v>134</v>
       </c>
-      <c r="C14" s="270"/>
+      <c r="C14" s="271"/>
       <c r="E14" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="F14" s="270" t="s">
+      <c r="F14" s="271" t="s">
         <v>115</v>
       </c>
-      <c r="G14" s="270"/>
+      <c r="G14" s="271"/>
       <c r="I14" s="57" t="s">
         <v>185</v>
       </c>
@@ -12238,17 +12557,17 @@
       <c r="A15" s="54" t="s">
         <v>139</v>
       </c>
-      <c r="B15" s="266" t="s">
+      <c r="B15" s="267" t="s">
         <v>135</v>
       </c>
-      <c r="C15" s="266"/>
+      <c r="C15" s="267"/>
       <c r="E15" s="49" t="s">
         <v>110</v>
       </c>
-      <c r="F15" s="266" t="s">
+      <c r="F15" s="267" t="s">
         <v>116</v>
       </c>
-      <c r="G15" s="266"/>
+      <c r="G15" s="267"/>
       <c r="I15" s="49" t="s">
         <v>186</v>
       </c>
@@ -12715,16 +13034,16 @@
       <c r="T5" s="28" t="s">
         <v>193</v>
       </c>
-      <c r="V5" s="265" t="s">
+      <c r="V5" s="266" t="s">
         <v>274</v>
       </c>
-      <c r="W5" s="265"/>
-      <c r="X5" s="265"/>
-      <c r="Y5" s="265"/>
-      <c r="Z5" s="265"/>
-      <c r="AA5" s="265"/>
-      <c r="AB5" s="265"/>
-      <c r="AC5" s="265"/>
+      <c r="W5" s="266"/>
+      <c r="X5" s="266"/>
+      <c r="Y5" s="266"/>
+      <c r="Z5" s="266"/>
+      <c r="AA5" s="266"/>
+      <c r="AB5" s="266"/>
+      <c r="AC5" s="266"/>
     </row>
     <row r="6" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="58" t="s">
@@ -12948,10 +13267,10 @@
       <c r="F9" s="97">
         <v>16</v>
       </c>
-      <c r="H9" s="265" t="s">
+      <c r="H9" s="266" t="s">
         <v>275</v>
       </c>
-      <c r="I9" s="265"/>
+      <c r="I9" s="266"/>
       <c r="K9" s="70">
         <v>192</v>
       </c>
@@ -13329,10 +13648,10 @@
       <c r="F15" s="96">
         <v>16</v>
       </c>
-      <c r="H15" s="265" t="s">
+      <c r="H15" s="266" t="s">
         <v>275</v>
       </c>
-      <c r="I15" s="265"/>
+      <c r="I15" s="266"/>
       <c r="K15" s="72">
         <v>172</v>
       </c>
@@ -13798,24 +14117,24 @@
       <c r="A1" s="120" t="s">
         <v>323</v>
       </c>
-      <c r="B1" s="271" t="s">
+      <c r="B1" s="284" t="s">
         <v>326</v>
       </c>
-      <c r="C1" s="272"/>
-      <c r="D1" s="272"/>
-      <c r="E1" s="273"/>
-      <c r="F1" s="274" t="s">
+      <c r="C1" s="285"/>
+      <c r="D1" s="285"/>
+      <c r="E1" s="286"/>
+      <c r="F1" s="287" t="s">
         <v>327</v>
       </c>
-      <c r="G1" s="275"/>
-      <c r="H1" s="275"/>
-      <c r="I1" s="276"/>
-      <c r="J1" s="286" t="s">
+      <c r="G1" s="288"/>
+      <c r="H1" s="288"/>
+      <c r="I1" s="289"/>
+      <c r="J1" s="272" t="s">
         <v>350</v>
       </c>
-      <c r="K1" s="287"/>
-      <c r="L1" s="287"/>
-      <c r="M1" s="288"/>
+      <c r="K1" s="273"/>
+      <c r="L1" s="273"/>
+      <c r="M1" s="274"/>
     </row>
     <row r="2" spans="1:13" s="105" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="50" t="s">
@@ -14000,18 +14319,18 @@
       <c r="E6" s="172" t="s">
         <v>401</v>
       </c>
-      <c r="F6" s="280" t="s">
+      <c r="F6" s="278" t="s">
         <v>343</v>
       </c>
-      <c r="G6" s="281"/>
-      <c r="H6" s="281"/>
-      <c r="I6" s="282"/>
-      <c r="J6" s="280" t="s">
+      <c r="G6" s="279"/>
+      <c r="H6" s="279"/>
+      <c r="I6" s="280"/>
+      <c r="J6" s="278" t="s">
         <v>343</v>
       </c>
-      <c r="K6" s="281"/>
-      <c r="L6" s="281"/>
-      <c r="M6" s="282"/>
+      <c r="K6" s="279"/>
+      <c r="L6" s="279"/>
+      <c r="M6" s="280"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="53" t="s">
@@ -14029,44 +14348,44 @@
       <c r="E7" s="175" t="s">
         <v>403</v>
       </c>
-      <c r="F7" s="283" t="s">
+      <c r="F7" s="281" t="s">
         <v>344</v>
       </c>
-      <c r="G7" s="284"/>
-      <c r="H7" s="284"/>
-      <c r="I7" s="285"/>
-      <c r="J7" s="283" t="s">
+      <c r="G7" s="282"/>
+      <c r="H7" s="282"/>
+      <c r="I7" s="283"/>
+      <c r="J7" s="281" t="s">
         <v>344</v>
       </c>
-      <c r="K7" s="284"/>
-      <c r="L7" s="284"/>
-      <c r="M7" s="285"/>
+      <c r="K7" s="282"/>
+      <c r="L7" s="282"/>
+      <c r="M7" s="283"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="54" t="s">
         <v>332</v>
       </c>
-      <c r="B8" s="277">
+      <c r="B8" s="275">
         <f>2^32</f>
         <v>4294967296</v>
       </c>
-      <c r="C8" s="278"/>
-      <c r="D8" s="278"/>
-      <c r="E8" s="279"/>
-      <c r="F8" s="277">
+      <c r="C8" s="276"/>
+      <c r="D8" s="276"/>
+      <c r="E8" s="277"/>
+      <c r="F8" s="275">
         <f>2^32</f>
         <v>4294967296</v>
       </c>
-      <c r="G8" s="278"/>
-      <c r="H8" s="278"/>
-      <c r="I8" s="279"/>
-      <c r="J8" s="277">
+      <c r="G8" s="276"/>
+      <c r="H8" s="276"/>
+      <c r="I8" s="277"/>
+      <c r="J8" s="275">
         <f>2^32</f>
         <v>4294967296</v>
       </c>
-      <c r="K8" s="278"/>
-      <c r="L8" s="278"/>
-      <c r="M8" s="279"/>
+      <c r="K8" s="276"/>
+      <c r="L8" s="276"/>
+      <c r="M8" s="277"/>
     </row>
     <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -14598,16 +14917,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="F7:I7"/>
     <mergeCell ref="J1:M1"/>
     <mergeCell ref="F8:I8"/>
     <mergeCell ref="J8:M8"/>
     <mergeCell ref="J6:M6"/>
     <mergeCell ref="J7:M7"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="F7:I7"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14639,14 +14958,14 @@
       <c r="A1" s="192" t="s">
         <v>350</v>
       </c>
-      <c r="B1" s="289" t="s">
+      <c r="B1" s="290" t="s">
         <v>420</v>
       </c>
-      <c r="C1" s="289"/>
-      <c r="D1" s="289"/>
-      <c r="E1" s="289"/>
-      <c r="F1" s="289"/>
-      <c r="G1" s="289"/>
+      <c r="C1" s="290"/>
+      <c r="D1" s="290"/>
+      <c r="E1" s="290"/>
+      <c r="F1" s="290"/>
+      <c r="G1" s="290"/>
     </row>
     <row r="3" spans="1:8" s="99" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="58" t="s">
@@ -15540,7 +15859,7 @@
   <dimension ref="A1:S28"/>
   <sheetViews>
     <sheetView topLeftCell="A3" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A3" sqref="A3"/>
       <selection pane="bottomLeft" activeCell="B12" sqref="B12:C12"/>
     </sheetView>
@@ -15569,14 +15888,14 @@
       <c r="A1" s="100" t="s">
         <v>548</v>
       </c>
-      <c r="B1" s="290" t="s">
+      <c r="B1" s="291" t="s">
         <v>549</v>
       </c>
-      <c r="C1" s="290"/>
-      <c r="D1" s="290"/>
-      <c r="E1" s="290"/>
-      <c r="F1" s="290"/>
-      <c r="G1" s="290"/>
+      <c r="C1" s="291"/>
+      <c r="D1" s="291"/>
+      <c r="E1" s="291"/>
+      <c r="F1" s="291"/>
+      <c r="G1" s="291"/>
       <c r="H1" s="199"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -15956,7 +16275,7 @@
       <c r="I16" s="202">
         <v>255255255128</v>
       </c>
-      <c r="J16" s="291" t="s">
+      <c r="J16" s="292" t="s">
         <v>621</v>
       </c>
       <c r="K16" s="196" t="s">
@@ -16012,7 +16331,7 @@
       <c r="I17" s="202">
         <v>255255255192</v>
       </c>
-      <c r="J17" s="291"/>
+      <c r="J17" s="292"/>
       <c r="K17" s="196" t="s">
         <v>603</v>
       </c>
@@ -16066,7 +16385,7 @@
       <c r="I18" s="207" t="s">
         <v>358</v>
       </c>
-      <c r="J18" s="291"/>
+      <c r="J18" s="292"/>
       <c r="K18" s="196" t="s">
         <v>339</v>
       </c>
@@ -16120,7 +16439,7 @@
       <c r="I19" s="208">
         <v>255255255128</v>
       </c>
-      <c r="J19" s="291"/>
+      <c r="J19" s="292"/>
       <c r="K19" s="196" t="s">
         <v>563</v>
       </c>
@@ -16417,16 +16736,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="292" t="s">
+      <c r="A1" s="293" t="s">
         <v>677</v>
       </c>
-      <c r="B1" s="292"/>
-      <c r="C1" s="292"/>
-      <c r="E1" s="292" t="s">
+      <c r="B1" s="293"/>
+      <c r="C1" s="293"/>
+      <c r="E1" s="293" t="s">
         <v>666</v>
       </c>
-      <c r="F1" s="292"/>
-      <c r="G1" s="292"/>
+      <c r="F1" s="293"/>
+      <c r="G1" s="293"/>
       <c r="I1" s="12" t="s">
         <v>643</v>
       </c>
@@ -16480,7 +16799,7 @@
       <c r="M2" s="222" t="s">
         <v>646</v>
       </c>
-      <c r="N2" s="293" t="s">
+      <c r="N2" s="294" t="s">
         <v>627</v>
       </c>
     </row>
@@ -16518,7 +16837,7 @@
       <c r="M3" s="224" t="s">
         <v>341</v>
       </c>
-      <c r="N3" s="293"/>
+      <c r="N3" s="294"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -16554,7 +16873,7 @@
       <c r="M4" s="227" t="s">
         <v>645</v>
       </c>
-      <c r="N4" s="294"/>
+      <c r="N4" s="295"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -16590,7 +16909,7 @@
       <c r="M5" s="231" t="s">
         <v>647</v>
       </c>
-      <c r="N5" s="295" t="s">
+      <c r="N5" s="296" t="s">
         <v>631</v>
       </c>
     </row>
@@ -16628,7 +16947,7 @@
       <c r="M6" s="227" t="s">
         <v>648</v>
       </c>
-      <c r="N6" s="296"/>
+      <c r="N6" s="297"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -16664,7 +16983,7 @@
       <c r="M7" s="224" t="s">
         <v>645</v>
       </c>
-      <c r="N7" s="297"/>
+      <c r="N7" s="298"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -16701,7 +17020,7 @@
       <c r="M8" s="236" t="s">
         <v>649</v>
       </c>
-      <c r="N8" s="298" t="s">
+      <c r="N8" s="299" t="s">
         <v>630</v>
       </c>
     </row>
@@ -16730,14 +17049,14 @@
       <c r="M9" s="224" t="s">
         <v>341</v>
       </c>
-      <c r="N9" s="299"/>
+      <c r="N9" s="300"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="289" t="s">
+      <c r="A10" s="290" t="s">
         <v>678</v>
       </c>
-      <c r="B10" s="289"/>
-      <c r="C10" s="289"/>
+      <c r="B10" s="290"/>
+      <c r="C10" s="290"/>
       <c r="E10" t="s">
         <v>659</v>
       </c>
@@ -16762,12 +17081,12 @@
       <c r="M10" s="240" t="s">
         <v>650</v>
       </c>
-      <c r="N10" s="300"/>
+      <c r="N10" s="301"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="289"/>
-      <c r="B11" s="289"/>
-      <c r="C11" s="289"/>
+      <c r="A11" s="290"/>
+      <c r="B11" s="290"/>
+      <c r="C11" s="290"/>
       <c r="E11" t="s">
         <v>205</v>
       </c>
@@ -16779,9 +17098,9 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="289"/>
-      <c r="B12" s="289"/>
-      <c r="C12" s="289"/>
+      <c r="A12" s="290"/>
+      <c r="B12" s="290"/>
+      <c r="C12" s="290"/>
       <c r="E12" t="s">
         <v>659</v>
       </c>
@@ -16793,9 +17112,9 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="289"/>
-      <c r="B13" s="289"/>
-      <c r="C13" s="289"/>
+      <c r="A13" s="290"/>
+      <c r="B13" s="290"/>
+      <c r="C13" s="290"/>
       <c r="E13" t="s">
         <v>652</v>
       </c>

</xml_diff>

<commit_message>
informacion capa de enlace y protocolos cdp lldp
</commit_message>
<xml_diff>
--- a/docs/protocols_suite.xlsx
+++ b/docs/protocols_suite.xlsx
@@ -5,16 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\networks\CISCO\saves\ccna2-mj14\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\networks\CISCO\saves\ccna2-mj14\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D1EA3BBD-85BC-4DF4-80AF-E5E95B665420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E4E998-D895-4EF1-8D21-E325E834FDA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="30" windowWidth="20460" windowHeight="10770" xr2:uid="{0A8DE5AC-929E-4116-BBBB-758591308C37}"/>
+    <workbookView xWindow="30" yWindow="30" windowWidth="20460" windowHeight="10770" activeTab="1" xr2:uid="{0A8DE5AC-929E-4116-BBBB-758591308C37}"/>
   </bookViews>
   <sheets>
-    <sheet name="AND" sheetId="1" r:id="rId1"/>
-    <sheet name="BIN" sheetId="2" r:id="rId2"/>
+    <sheet name="UNIDADES" sheetId="3" r:id="rId1"/>
+    <sheet name="ENLACE" sheetId="4" r:id="rId2"/>
+    <sheet name="AND" sheetId="1" r:id="rId3"/>
+    <sheet name="BIN" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="162">
   <si>
     <t>AND</t>
   </si>
@@ -336,6 +338,323 @@
   <si>
     <t>10100111</t>
   </si>
+  <si>
+    <t>ALMACENAMIENTO</t>
+  </si>
+  <si>
+    <t>ANCHO DE BANDA</t>
+  </si>
+  <si>
+    <t>FRECUENCIA</t>
+  </si>
+  <si>
+    <t>Binary Digit</t>
+  </si>
+  <si>
+    <t>1 | 0</t>
+  </si>
+  <si>
+    <t>Byte</t>
+  </si>
+  <si>
+    <t>bps</t>
+  </si>
+  <si>
+    <t>bits por segundo</t>
+  </si>
+  <si>
+    <t>10^0</t>
+  </si>
+  <si>
+    <t>Hertz</t>
+  </si>
+  <si>
+    <t>ciclo por segundo</t>
+  </si>
+  <si>
+    <t>8 bits</t>
+  </si>
+  <si>
+    <t>KyloByte</t>
+  </si>
+  <si>
+    <t>MegaByte</t>
+  </si>
+  <si>
+    <t>10^3</t>
+  </si>
+  <si>
+    <t>10^6</t>
+  </si>
+  <si>
+    <t>10^9</t>
+  </si>
+  <si>
+    <t>10^12</t>
+  </si>
+  <si>
+    <t>10^15</t>
+  </si>
+  <si>
+    <t>10^18</t>
+  </si>
+  <si>
+    <t>10^21</t>
+  </si>
+  <si>
+    <t>10^24</t>
+  </si>
+  <si>
+    <t>10^27</t>
+  </si>
+  <si>
+    <t>10^30</t>
+  </si>
+  <si>
+    <t>10^33</t>
+  </si>
+  <si>
+    <t>GigaByte</t>
+  </si>
+  <si>
+    <t>TeraByte</t>
+  </si>
+  <si>
+    <t>PetaByte</t>
+  </si>
+  <si>
+    <t>ExaByte</t>
+  </si>
+  <si>
+    <t>ZettaByte</t>
+  </si>
+  <si>
+    <t>YottaByte</t>
+  </si>
+  <si>
+    <t>BrontoByte</t>
+  </si>
+  <si>
+    <t>GeopByte</t>
+  </si>
+  <si>
+    <t>SaganByte</t>
+  </si>
+  <si>
+    <t>1000B</t>
+  </si>
+  <si>
+    <t>1000KB</t>
+  </si>
+  <si>
+    <t>1000MB</t>
+  </si>
+  <si>
+    <t>1000GB</t>
+  </si>
+  <si>
+    <t>1000TB</t>
+  </si>
+  <si>
+    <t>1000PB</t>
+  </si>
+  <si>
+    <t>1000XB</t>
+  </si>
+  <si>
+    <t>1000ZB</t>
+  </si>
+  <si>
+    <t>1000YB</t>
+  </si>
+  <si>
+    <t>1000BB</t>
+  </si>
+  <si>
+    <t>1000GeB</t>
+  </si>
+  <si>
+    <t>Unidad</t>
+  </si>
+  <si>
+    <t>Equiv</t>
+  </si>
+  <si>
+    <t>Exp</t>
+  </si>
+  <si>
+    <t>Real</t>
+  </si>
+  <si>
+    <t>KiB</t>
+  </si>
+  <si>
+    <t>MiB</t>
+  </si>
+  <si>
+    <t>GiB</t>
+  </si>
+  <si>
+    <t>TiB</t>
+  </si>
+  <si>
+    <t>PiB</t>
+  </si>
+  <si>
+    <t>EiB</t>
+  </si>
+  <si>
+    <t>ZiB</t>
+  </si>
+  <si>
+    <t>YiB</t>
+  </si>
+  <si>
+    <t>BiB</t>
+  </si>
+  <si>
+    <t>SiB</t>
+  </si>
+  <si>
+    <t>GeiB</t>
+  </si>
+  <si>
+    <t>sufijo bi</t>
+  </si>
+  <si>
+    <t>Kbps</t>
+  </si>
+  <si>
+    <t>Mbps</t>
+  </si>
+  <si>
+    <t>Gbps</t>
+  </si>
+  <si>
+    <t>Tbps</t>
+  </si>
+  <si>
+    <t>1000bps</t>
+  </si>
+  <si>
+    <t>1000Kbps</t>
+  </si>
+  <si>
+    <t>1000Gbps</t>
+  </si>
+  <si>
+    <t>1000Mbps</t>
+  </si>
+  <si>
+    <t>Khz</t>
+  </si>
+  <si>
+    <t>Mhz</t>
+  </si>
+  <si>
+    <t>Ghz</t>
+  </si>
+  <si>
+    <t>Descripcion</t>
+  </si>
+  <si>
+    <t>HALF</t>
+  </si>
+  <si>
+    <t>FULL</t>
+  </si>
+  <si>
+    <t>Simplex</t>
+  </si>
+  <si>
+    <t>Full Full</t>
+  </si>
+  <si>
+    <t>Duplex</t>
+  </si>
+  <si>
+    <t>uno envia el resto recibe datos</t>
+  </si>
+  <si>
+    <t>El host envia o recibe datos</t>
+  </si>
+  <si>
+    <t>El host envia y recibe datos</t>
+  </si>
+  <si>
+    <t>Varios envian y reciben datos</t>
+  </si>
+  <si>
+    <t>Colision</t>
+  </si>
+  <si>
+    <t>Funcionamiento</t>
+  </si>
+  <si>
+    <t>Limitado a su configuracion Base (cantidad de puertos fisicos)</t>
+  </si>
+  <si>
+    <t>Permiten la incorporacion de mas interfaces de ser necesario</t>
+  </si>
+  <si>
+    <t>Utilizan un conector para funcionar como uno de mayor capacidad</t>
+  </si>
+  <si>
+    <t>Reenvia las tramas apenas identifique la direccion de destino</t>
+  </si>
+  <si>
+    <t>Almacena las tramas en un buffer y las reenvia al verificarlas</t>
+  </si>
+  <si>
+    <t>Reenvia las tramas tras leer los primeros 64Bytes</t>
+  </si>
+  <si>
+    <t>Fija</t>
+  </si>
+  <si>
+    <t>Expandible</t>
+  </si>
+  <si>
+    <t>Apilable</t>
+  </si>
+  <si>
+    <t>Config</t>
+  </si>
+  <si>
+    <t>Store-N-Forward (Almacen y Envio)</t>
+  </si>
+  <si>
+    <t>Fragment-Free  
+(Libre de Fragmentos)</t>
+  </si>
+  <si>
+    <t>Cut-Through 
+(Metodo de Corte)</t>
+  </si>
+  <si>
+    <t>Runt Frames</t>
+  </si>
+  <si>
+    <t>Giant Frames</t>
+  </si>
+  <si>
+    <t>CRC Frames</t>
+  </si>
+  <si>
+    <t>Throttle Frames</t>
+  </si>
+  <si>
+    <t>Tramas menores a 64 Bytes</t>
+  </si>
+  <si>
+    <t>Tramas mayores a 1500Bytes</t>
+  </si>
+  <si>
+    <t>Tramas descartadas por desbordamiento</t>
+  </si>
+  <si>
+    <t>Tramas que no superan la verificacion</t>
+  </si>
 </sst>
 </file>
 
@@ -377,7 +696,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -390,8 +709,14 @@
         <bgColor theme="4" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -482,11 +807,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -507,9 +861,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -521,221 +872,115 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="28">
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
+      <border outline="0">
         <top style="thin">
-          <color indexed="64"/>
+          <color theme="4" tint="0.39997558519241921"/>
         </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
-          <color indexed="64"/>
+          <color theme="4" tint="0.39997558519241921"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
+      <border outline="0">
         <top style="thin">
-          <color indexed="64"/>
+          <color theme="4" tint="0.39997558519241921"/>
         </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -744,6 +989,218 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -771,32 +1228,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{13D155E4-D398-407B-AC95-045F9D5206EB}" name="Tabla2" displayName="Tabla2" ref="A1:F5" totalsRowShown="0">
-  <autoFilter ref="A1:F5" xr:uid="{13D155E4-D398-407B-AC95-045F9D5206EB}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{E7414CB7-1FED-4FD4-8297-2BDCED5D1DE8}" name="AND"/>
-    <tableColumn id="2" xr3:uid="{923BA942-2940-46F1-A600-E4BB020F3A58}" name="DECIMAL"/>
-    <tableColumn id="3" xr3:uid="{0DC99166-0D88-49DF-9B1B-28434A4B74F0}" name="BYTE 1" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{ABF9CAD8-A787-4B66-8B8A-C0C4366DE6D0}" name="BYTE 2" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{61208B89-8C49-40A6-AE92-9D58A6E5E454}" name="BYTE 3" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{38B4EA60-9A9E-4313-BBBE-9937D44CFF29}" name="BYTE 4" dataDxfId="12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{BD40C91C-7D68-452F-89D9-0BC004F4C381}" name="Tabla4" displayName="Tabla4" ref="A4:D16" totalsRowShown="0">
+  <autoFilter ref="A4:D16" xr:uid="{BD40C91C-7D68-452F-89D9-0BC004F4C381}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{A3BB5F92-8FE1-4452-AF0C-3ED0E5F42C03}" name="Unidad"/>
+    <tableColumn id="2" xr3:uid="{941302C2-204B-41B1-A39A-A99F78D2D1CB}" name="Equiv"/>
+    <tableColumn id="3" xr3:uid="{78BF88C5-C612-405B-BE2C-3695F993B504}" name="Exp"/>
+    <tableColumn id="4" xr3:uid="{F9112DAA-1C09-4EE7-AE40-4C536DD30812}" name="Real"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{C9AF53D7-A713-40F6-9C94-063C8F914C37}" name="Tabla6" displayName="Tabla6" ref="K1:L3" totalsRowShown="0">
-  <autoFilter ref="K1:L3" xr:uid="{C9AF53D7-A713-40F6-9C94-063C8F914C37}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{8B32B56C-53AE-4DA3-B7C1-071C1812C674}" name="Porcion"/>
-    <tableColumn id="2" xr3:uid="{AFE0F479-AF1D-4714-A072-E70A82D15203}" name="Bit"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{C83D29F0-F075-4AAA-B25A-08ED3DC4158B}" name="Tabla7" displayName="Tabla7" ref="H1:I5" totalsRowShown="0">
   <autoFilter ref="H1:I5" xr:uid="{C83D29F0-F075-4AAA-B25A-08ED3DC4158B}"/>
   <tableColumns count="2">
@@ -807,30 +1251,124 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{04BE53F9-C997-49DA-B179-51E46754BDD7}" name="Tabla1" displayName="Tabla1" ref="A1:I3" totalsRowShown="0" headerRowDxfId="0">
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{04BE53F9-C997-49DA-B179-51E46754BDD7}" name="Tabla1" displayName="Tabla1" ref="A1:I3" totalsRowShown="0" headerRowDxfId="23">
   <autoFilter ref="A1:I3" xr:uid="{04BE53F9-C997-49DA-B179-51E46754BDD7}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{45E42E80-691C-4658-9C7A-825EAB495BDB}" name="EXP" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{7A68EA22-0E6C-4EA3-BCBD-6C63BB692668}" name="2^7" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{BB76D7D6-83F7-4051-BB82-13E817C5F251}" name="2^6" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{444E06F8-A657-4F80-B21B-8E02642777CF}" name="2^5" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{C84D46EF-0237-4529-9A12-0578060BDE3B}" name="2^4" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{51640218-50B5-44F3-A633-6D2B82581E6A}" name="2^3" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{86B4A6AB-87FF-4178-BD3A-A013F68C2BBD}" name="2^2" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{909C26AC-DCCD-4C35-ACD6-66F843B16D02}" name="2^1" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{51FD7346-8278-4121-8115-2A10C868B914}" name="2^0" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{45E42E80-691C-4658-9C7A-825EAB495BDB}" name="EXP" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{7A68EA22-0E6C-4EA3-BCBD-6C63BB692668}" name="2^7" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{BB76D7D6-83F7-4051-BB82-13E817C5F251}" name="2^6" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{444E06F8-A657-4F80-B21B-8E02642777CF}" name="2^5" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{C84D46EF-0237-4529-9A12-0578060BDE3B}" name="2^4" dataDxfId="18"/>
+    <tableColumn id="6" xr3:uid="{51640218-50B5-44F3-A633-6D2B82581E6A}" name="2^3" dataDxfId="17"/>
+    <tableColumn id="7" xr3:uid="{86B4A6AB-87FF-4178-BD3A-A013F68C2BBD}" name="2^2" dataDxfId="16"/>
+    <tableColumn id="8" xr3:uid="{909C26AC-DCCD-4C35-ACD6-66F843B16D02}" name="2^1" dataDxfId="15"/>
+    <tableColumn id="9" xr3:uid="{51FD7346-8278-4121-8115-2A10C868B914}" name="2^0" dataDxfId="14"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C0921313-5194-4281-912E-0CD6F3BE319F}" name="Tabla3" displayName="Tabla3" ref="K1:L10" totalsRowShown="0">
+  <autoFilter ref="K1:L10" xr:uid="{C0921313-5194-4281-912E-0CD6F3BE319F}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{3728F07D-C07B-43B6-846F-B73B5EC9C8A3}" name="DEC" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{6DDB2D9E-8B4C-46A8-A2AE-67B9AE9D2651}" name="BIN" dataDxfId="12"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{3EF010CC-D4C0-436D-B264-B8CC57A5128B}" name="Tabla5" displayName="Tabla5" ref="F12:H16" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="11">
+  <autoFilter ref="F12:H16" xr:uid="{3EF010CC-D4C0-436D-B264-B8CC57A5128B}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{1F9AE69C-28EF-4CF1-A461-0D1C91B52766}" name="Unidad"/>
+    <tableColumn id="2" xr3:uid="{3044743A-E847-41C4-AF9B-80138B0E36D5}" name="Equiv"/>
+    <tableColumn id="3" xr3:uid="{1B1C1B56-D99B-4E1F-98A2-9FE8100CAF40}" name="Exp"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{AD251824-3B13-4795-B35F-417484E7AF69}" name="Tabla8" displayName="Tabla8" ref="F4:H9" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="8">
+  <autoFilter ref="F4:H9" xr:uid="{AD251824-3B13-4795-B35F-417484E7AF69}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{F28365EC-BD0A-44CD-B5EA-CB6F0BCCDAD4}" name="Unidad"/>
+    <tableColumn id="2" xr3:uid="{5A1ED304-F3CA-4229-BAC6-0FA062A26E26}" name="Equiv"/>
+    <tableColumn id="3" xr3:uid="{9D70656F-A425-41E9-BC24-7094EDE7A56D}" name="Exp"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{E3EEB79C-8679-433C-8C8C-3BFCF027EE3C}" name="Tabla9" displayName="Tabla9" ref="A1:B5" totalsRowShown="0">
+  <autoFilter ref="A1:B5" xr:uid="{E3EEB79C-8679-433C-8C8C-3BFCF027EE3C}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{47B91FB0-7916-4C4D-9F1A-1F50E740BEB5}" name="Duplex"/>
+    <tableColumn id="2" xr3:uid="{B5310B13-F8D3-4239-9B35-D5E08F031862}" name="Descripcion"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C0921313-5194-4281-912E-0CD6F3BE319F}" name="Tabla3" displayName="Tabla3" ref="K1:L10" totalsRowShown="0">
-  <autoFilter ref="K1:L10" xr:uid="{C0921313-5194-4281-912E-0CD6F3BE319F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{4EA0A95F-0A9A-42FB-B81F-D3BDDE76DDCF}" name="Tabla10" displayName="Tabla10" ref="A7:B10" totalsRowShown="0" dataDxfId="3">
+  <autoFilter ref="A7:B10" xr:uid="{4EA0A95F-0A9A-42FB-B81F-D3BDDE76DDCF}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{3728F07D-C07B-43B6-846F-B73B5EC9C8A3}" name="DEC" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{6DDB2D9E-8B4C-46A8-A2AE-67B9AE9D2651}" name="BIN" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{AB57D7D5-2286-4A13-8513-64A4C83A1BB2}" name="Config" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{715E714A-BC19-407F-8767-A697EFF0C87F}" name="Descripcion" dataDxfId="4"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{E4A4F5A5-4AD8-4B75-87E2-1FCE48A09B58}" name="Tabla11" displayName="Tabla11" ref="D7:E10" totalsRowShown="0" dataDxfId="0">
+  <autoFilter ref="D7:E10" xr:uid="{E4A4F5A5-4AD8-4B75-87E2-1FCE48A09B58}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{0D3F5B5C-61F7-4E33-9A0A-85CA0329F28C}" name="Funcionamiento" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{158DBA94-D8E6-4A42-A591-57ED0B2D657F}" name="Descripcion" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{C510F25F-478A-459D-9915-9CDDA944B643}" name="Tabla12" displayName="Tabla12" ref="D1:E5" totalsRowShown="0">
+  <autoFilter ref="D1:E5" xr:uid="{C510F25F-478A-459D-9915-9CDDA944B643}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{3E24E882-2923-4716-AFD9-8025B0C1D532}" name="Colision"/>
+    <tableColumn id="2" xr3:uid="{107BC76E-6748-4D59-8FEB-63D73021E814}" name="Descripcion"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{13D155E4-D398-407B-AC95-045F9D5206EB}" name="Tabla2" displayName="Tabla2" ref="A1:F5" totalsRowShown="0">
+  <autoFilter ref="A1:F5" xr:uid="{13D155E4-D398-407B-AC95-045F9D5206EB}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{E7414CB7-1FED-4FD4-8297-2BDCED5D1DE8}" name="AND"/>
+    <tableColumn id="2" xr3:uid="{923BA942-2940-46F1-A600-E4BB020F3A58}" name="DECIMAL"/>
+    <tableColumn id="3" xr3:uid="{0DC99166-0D88-49DF-9B1B-28434A4B74F0}" name="BYTE 1" dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{ABF9CAD8-A787-4B66-8B8A-C0C4366DE6D0}" name="BYTE 2" dataDxfId="26"/>
+    <tableColumn id="5" xr3:uid="{61208B89-8C49-40A6-AE92-9D58A6E5E454}" name="BYTE 3" dataDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{38B4EA60-9A9E-4313-BBBE-9937D44CFF29}" name="BYTE 4" dataDxfId="24"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{C9AF53D7-A713-40F6-9C94-063C8F914C37}" name="Tabla6" displayName="Tabla6" ref="K1:L3" totalsRowShown="0">
+  <autoFilter ref="K1:L3" xr:uid="{C9AF53D7-A713-40F6-9C94-063C8F914C37}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{8B32B56C-53AE-4DA3-B7C1-071C1812C674}" name="Porcion"/>
+    <tableColumn id="2" xr3:uid="{AFE0F479-AF1D-4714-A072-E70A82D15203}" name="Bit"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1132,14 +1670,517 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1C0D167-B099-4BC2-A3E5-D097A8CFF4F1}">
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView topLeftCell="E4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="F3" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4" t="s">
+        <v>105</v>
+      </c>
+      <c r="F4" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="G4" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="H4" s="31" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" t="s">
+        <v>117</v>
+      </c>
+      <c r="F5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" t="s">
+        <v>106</v>
+      </c>
+      <c r="F6" t="s">
+        <v>118</v>
+      </c>
+      <c r="G6" t="s">
+        <v>122</v>
+      </c>
+      <c r="H6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F7" t="s">
+        <v>119</v>
+      </c>
+      <c r="G7" t="s">
+        <v>123</v>
+      </c>
+      <c r="H7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" t="s">
+        <v>108</v>
+      </c>
+      <c r="F8" t="s">
+        <v>120</v>
+      </c>
+      <c r="G8" t="s">
+        <v>125</v>
+      </c>
+      <c r="H8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="F9" t="s">
+        <v>121</v>
+      </c>
+      <c r="G9" t="s">
+        <v>124</v>
+      </c>
+      <c r="H9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D11" t="s">
+        <v>111</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B12" t="s">
+        <v>97</v>
+      </c>
+      <c r="C12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" t="s">
+        <v>112</v>
+      </c>
+      <c r="F12" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="G12" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="H12" s="31" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="F13" t="s">
+        <v>66</v>
+      </c>
+      <c r="G13" t="s">
+        <v>67</v>
+      </c>
+      <c r="H13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>88</v>
+      </c>
+      <c r="B14" t="s">
+        <v>99</v>
+      </c>
+      <c r="C14" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" t="s">
+        <v>114</v>
+      </c>
+      <c r="F14" t="s">
+        <v>126</v>
+      </c>
+      <c r="G14" t="s">
+        <v>122</v>
+      </c>
+      <c r="H14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>89</v>
+      </c>
+      <c r="B15" t="s">
+        <v>100</v>
+      </c>
+      <c r="C15" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" t="s">
+        <v>116</v>
+      </c>
+      <c r="F15" t="s">
+        <v>127</v>
+      </c>
+      <c r="G15" t="s">
+        <v>123</v>
+      </c>
+      <c r="H15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>90</v>
+      </c>
+      <c r="B16" t="s">
+        <v>101</v>
+      </c>
+      <c r="C16" t="s">
+        <v>81</v>
+      </c>
+      <c r="D16" t="s">
+        <v>115</v>
+      </c>
+      <c r="F16" t="s">
+        <v>128</v>
+      </c>
+      <c r="G16" t="s">
+        <v>125</v>
+      </c>
+      <c r="H16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="A3:D3"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="3">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91814D92-A16C-42E0-8C0D-DAD67E9661CC}">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" customWidth="1"/>
+    <col min="3" max="3" width="2.85546875" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G1" t="s">
+        <v>139</v>
+      </c>
+      <c r="H1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D3" t="s">
+        <v>155</v>
+      </c>
+      <c r="E3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D4" t="s">
+        <v>157</v>
+      </c>
+      <c r="E4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5" t="s">
+        <v>138</v>
+      </c>
+      <c r="D5" t="s">
+        <v>156</v>
+      </c>
+      <c r="E5" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>150</v>
+      </c>
+      <c r="B7" t="s">
+        <v>129</v>
+      </c>
+      <c r="D7" t="s">
+        <v>140</v>
+      </c>
+      <c r="E7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>153</v>
+      </c>
+      <c r="E8" s="32" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="32" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>142</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>151</v>
+      </c>
+      <c r="E9" s="32" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="32" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="32" t="s">
+        <v>149</v>
+      </c>
+      <c r="B10" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="D10" s="32" t="s">
+        <v>152</v>
+      </c>
+      <c r="E10" s="32" t="s">
+        <v>146</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="4">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDCDC4A6-1EF1-4C78-A9DD-CA43A0BDED74}">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1304,12 +2345,12 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="27"/>
+      <c r="A6" s="23"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="26"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
@@ -1318,16 +2359,16 @@
       <c r="B7" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="F7" s="17" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1335,19 +2376,19 @@
       <c r="A8" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="19">
+      <c r="B8" s="18">
         <v>255255255248</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="21" t="s">
+      <c r="F8" s="20" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1358,16 +2399,16 @@
       <c r="B9" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="F9" s="17" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1378,16 +2419,16 @@
       <c r="B10" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="D10" s="22" t="s">
+      <c r="D10" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="E10" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="F10" s="23" t="s">
+      <c r="F10" s="22" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1405,13 +2446,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EE4E250-59DA-4DBD-983A-B016C4E5B6E6}">
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4:I4"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="B2:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1532,16 +2573,16 @@
       <c r="A4" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="16">
+      <c r="B4" s="27">
         <v>200</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
       <c r="K4" s="3">
         <v>192</v>
       </c>

</xml_diff>